<commit_message>
Added Extent Report and Zip Report
</commit_message>
<xml_diff>
--- a/src/TestData/Add_Appointment_Suite.xlsx
+++ b/src/TestData/Add_Appointment_Suite.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="258">
   <si>
     <t>Browser</t>
   </si>
@@ -791,47 +791,19 @@
     <t>S5</t>
   </si>
   <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t>FAIL Object not found Unable to locate element: {"method":"xpath","selector":".//*[@id='todayAppointmentsContainer']/div[1]/h2"}
-Command duration or timeout: 10.08 seconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: '2.53.1', revision: 'a36b8b1', time: '2016-06-30 17:32:46'
-System info: host: 'DESKTOP-6G2G9OB', ip: '192.168.1.203', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_111'
-Driver info: org.openqa.selenium.firefox.FirefoxDriver
-Capabilities [{applicationCacheEnabled=true, rotatable=false, handlesAlerts=true, databaseEnabled=true, version=47.0.1, platform=WINDOWS, nativeEvents=false, acceptSslCerts=true, webStorageEnabled=true, locationContextEnabled=true, browserName=firefox, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true}]
-Session ID: 1f5e7048-4c01-4bea-8555-c47b1f76fe7d
-*** Element info: {Using=xpath, value=.//*[@id='todayAppointmentsContainer']/div[1]/h2}</t>
-  </si>
-  <si>
-    <t>FAIL Object not found Unable to locate element: {"method":"xpath","selector":".//*[@id='todayAppointmentsContainer']/div[1]/h2"}
-Command duration or timeout: 10.06 seconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: '2.53.1', revision: 'a36b8b1', time: '2016-06-30 17:32:46'
-System info: host: 'DESKTOP-6G2G9OB', ip: '192.168.1.203', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_111'
-Driver info: org.openqa.selenium.firefox.FirefoxDriver
-Capabilities [{applicationCacheEnabled=true, rotatable=false, handlesAlerts=true, databaseEnabled=true, version=47.0.1, platform=WINDOWS, nativeEvents=false, acceptSslCerts=true, webStorageEnabled=true, locationContextEnabled=true, browserName=firefox, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true}]
-Session ID: 8cf17b7b-80b8-4a10-aa73-ba1909fbdee9
-*** Element info: {Using=xpath, value=.//*[@id='todayAppointmentsContainer']/div[1]/h2}</t>
-  </si>
-  <si>
-    <t>FAIL Object not found Unable to locate element: {"method":"xpath","selector":".//*[@id='todayAppointmentsContainer']/div[1]/h2"}
-Command duration or timeout: 10.05 seconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: '2.53.1', revision: 'a36b8b1', time: '2016-06-30 17:32:46'
-System info: host: 'DESKTOP-6G2G9OB', ip: '192.168.1.204', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_111'
-Driver info: org.openqa.selenium.firefox.FirefoxDriver
-Capabilities [{applicationCacheEnabled=true, rotatable=false, handlesAlerts=true, databaseEnabled=true, version=47.0.1, platform=WINDOWS, nativeEvents=false, acceptSslCerts=true, webStorageEnabled=true, locationContextEnabled=true, browserName=firefox, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true}]
-Session ID: 92732a46-0314-45fe-a204-fb165b337c4e
-*** Element info: {Using=xpath, value=.//*[@id='todayAppointmentsContainer']/div[1]/h2}</t>
+    <t>Logging into PRM</t>
+  </si>
+  <si>
+    <t>Navigate to test url</t>
+  </si>
+  <si>
+    <t>Navigate to google.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="19">
     <font>
       <sz val="10"/>
@@ -945,7 +917,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1050,6 +1022,12 @@
         <fgColor indexed="55"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -1106,7 +1084,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1200,9 +1178,6 @@
     <xf numFmtId="0" fontId="15" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1216,6 +1191,12 @@
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1519,10 +1500,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="25.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="61.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="16.28515625" collapsed="true"/>
-    <col min="4" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="25.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="61.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" customHeight="1">
@@ -1952,19 +1933,19 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="10.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="23.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="43.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="13.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="17.0" collapsed="true"/>
-    <col min="8" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="10.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="43.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="22.5" customHeight="1">
@@ -2001,7 +1982,7 @@
         <v>229</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>74</v>
+        <v>255</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>13</v>
@@ -2024,10 +2005,10 @@
         <v>234</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>74</v>
+        <v>257</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F3" s="18" t="s">
         <v>74</v>
@@ -2096,7 +2077,7 @@
         <v>74</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
@@ -2115,78 +2096,78 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V334"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="44" width="11.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="44" width="9.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="44" width="6.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="44" width="29.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="44" width="23.42578125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="44" width="25.7109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="44" width="31.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="44" width="255.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="44" width="6.85546875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="44" width="16.28515625" collapsed="true"/>
-    <col min="11" max="11" style="44" width="9.140625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="44" width="10.42578125" collapsed="true"/>
-    <col min="13" max="15" bestFit="true" customWidth="true" style="44" width="7.5703125" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" style="44" width="3.0" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" hidden="true" style="44" width="7.5703125" collapsed="true"/>
-    <col min="18" max="19" customWidth="true" style="44" width="13.85546875" collapsed="true"/>
-    <col min="20" max="21" bestFit="true" customWidth="true" style="44" width="32.42578125" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="44" width="7.5703125" collapsed="true"/>
-    <col min="23" max="16384" style="44" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="11.140625" style="44" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.5703125" style="44" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.7109375" style="44" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="29" style="44" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.42578125" style="44" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="25.7109375" style="44" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="31.28515625" style="44" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.7109375" style="45" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="6.85546875" style="44" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.28515625" style="44" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.140625" style="44" collapsed="1"/>
+    <col min="12" max="12" width="10.42578125" style="44" customWidth="1" collapsed="1"/>
+    <col min="13" max="15" width="7.5703125" style="44" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="3" style="44" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="7.5703125" style="44" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="19" width="13.85546875" style="44" customWidth="1" collapsed="1"/>
+    <col min="20" max="21" width="32.42578125" style="44" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="7.5703125" style="44" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="16384" width="9.140625" style="44" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="56" customFormat="1">
-      <c r="A1" s="55" t="s">
+    <row r="1" spans="1:22" s="55" customFormat="1">
+      <c r="A1" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="55" t="s">
+      <c r="C1" s="54" t="s">
         <v>141</v>
       </c>
-      <c r="D1" s="55" t="s">
+      <c r="D1" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="55" t="s">
+      <c r="E1" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="55" t="s">
+      <c r="F1" s="54" t="s">
         <v>165</v>
       </c>
-      <c r="G1" s="55" t="s">
+      <c r="G1" s="54" t="s">
         <v>104</v>
       </c>
-      <c r="H1" s="55" t="s">
+      <c r="H1" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="55" t="s">
+      <c r="I1" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="56" t="s">
+      <c r="J1" s="55" t="s">
         <v>145</v>
       </c>
-      <c r="K1" s="56" t="s">
+      <c r="K1" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="57"/>
-      <c r="O1" s="57"/>
-      <c r="P1" s="57"/>
-      <c r="Q1" s="57"/>
-      <c r="R1" s="57"/>
-      <c r="S1" s="57"/>
-      <c r="T1" s="58"/>
-      <c r="U1" s="59"/>
-      <c r="V1" s="60"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="58"/>
+      <c r="V1" s="59"/>
     </row>
     <row r="2" spans="1:22" s="45" customFormat="1">
       <c r="A2" s="45" t="s">
@@ -2203,9 +2184,6 @@
       </c>
       <c r="F2" s="45" t="s">
         <v>170</v>
-      </c>
-      <c r="H2" s="51" t="s">
-        <v>255</v>
       </c>
       <c r="I2" s="45" t="s">
         <v>74</v>
@@ -2244,9 +2222,6 @@
       <c r="F3" s="45" t="s">
         <v>173</v>
       </c>
-      <c r="H3" s="51" t="s">
-        <v>255</v>
-      </c>
       <c r="I3" s="45" t="s">
         <v>74</v>
       </c>
@@ -2287,9 +2262,6 @@
       <c r="G4" s="45" t="s">
         <v>174</v>
       </c>
-      <c r="H4" s="51" t="s">
-        <v>255</v>
-      </c>
       <c r="I4" s="45" t="s">
         <v>74</v>
       </c>
@@ -2327,9 +2299,6 @@
       <c r="G5" s="45" t="s">
         <v>175</v>
       </c>
-      <c r="H5" s="51" t="s">
-        <v>255</v>
-      </c>
       <c r="I5" s="45" t="s">
         <v>74</v>
       </c>
@@ -2362,9 +2331,6 @@
       <c r="G6" s="45" t="s">
         <v>176</v>
       </c>
-      <c r="H6" s="51" t="s">
-        <v>255</v>
-      </c>
       <c r="K6" s="45" t="s">
         <v>13</v>
       </c>
@@ -2390,9 +2356,6 @@
       <c r="F7" s="45" t="s">
         <v>246</v>
       </c>
-      <c r="H7" s="51" t="s">
-        <v>255</v>
-      </c>
       <c r="K7" s="45" t="s">
         <v>13</v>
       </c>
@@ -2424,9 +2387,6 @@
       <c r="G8" s="45" t="s">
         <v>248</v>
       </c>
-      <c r="H8" s="51" t="s">
-        <v>258</v>
-      </c>
       <c r="K8" s="45" t="s">
         <v>13</v>
       </c>
@@ -2439,23 +2399,26 @@
       <c r="U8" s="51"/>
       <c r="V8" s="51"/>
     </row>
-    <row r="9" spans="1:22" s="46" customFormat="1">
-      <c r="A9" s="46" t="s">
-        <v>93</v>
-      </c>
-      <c r="C9" s="45">
+    <row r="9" spans="1:22" s="60" customFormat="1">
+      <c r="A9" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="60">
         <v>8</v>
       </c>
-      <c r="E9" s="46" t="s">
+      <c r="D9" s="60" t="s">
+        <v>256</v>
+      </c>
+      <c r="E9" s="60" t="s">
         <v>167</v>
       </c>
-      <c r="F9" s="46" t="s">
+      <c r="F9" s="60" t="s">
         <v>232</v>
       </c>
-      <c r="K9" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="N9" s="53"/>
+      <c r="K9" s="60" t="s">
+        <v>13</v>
+      </c>
+      <c r="N9" s="61"/>
     </row>
     <row r="10" spans="1:22" s="46" customFormat="1">
       <c r="A10" s="46" t="s">
@@ -2470,12 +2433,12 @@
       <c r="F10" s="46" t="s">
         <v>233</v>
       </c>
-      <c r="H10" s="53"/>
+      <c r="H10" s="45"/>
       <c r="K10" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="R10" s="54"/>
-      <c r="S10" s="54"/>
+      <c r="R10" s="53"/>
+      <c r="S10" s="53"/>
     </row>
     <row r="11" spans="1:22" s="46" customFormat="1">
       <c r="A11" s="46" t="s">
@@ -2490,353 +2453,993 @@
       <c r="G11" s="46" t="s">
         <v>236</v>
       </c>
-      <c r="H11"/>
+      <c r="H11" s="45"/>
       <c r="K11" s="46" t="s">
-        <v>13</v>
-      </c>
-      <c r="R11" s="54"/>
-      <c r="S11" s="54"/>
+        <v>8</v>
+      </c>
+      <c r="R11" s="53"/>
+      <c r="S11" s="53"/>
     </row>
     <row r="12" spans="1:22" s="47" customFormat="1">
-      <c r="H12" s="48"/>
+      <c r="H12" s="45"/>
       <c r="I12" s="48"/>
       <c r="J12" s="48"/>
       <c r="K12" s="48"/>
       <c r="L12" s="48"/>
       <c r="M12" s="48"/>
     </row>
-    <row r="13" spans="1:22" s="47" customFormat="1"/>
-    <row r="14" spans="1:22" s="47" customFormat="1"/>
+    <row r="13" spans="1:22" s="47" customFormat="1">
+      <c r="H13" s="45"/>
+    </row>
+    <row r="14" spans="1:22" s="47" customFormat="1">
+      <c r="H14" s="45"/>
+    </row>
     <row r="15" spans="1:22" s="47" customFormat="1">
       <c r="E15" s="52"/>
+      <c r="H15" s="45"/>
     </row>
     <row r="16" spans="1:22" s="47" customFormat="1">
       <c r="E16" s="52"/>
-    </row>
-    <row r="17" spans="6:7" s="47" customFormat="1"/>
-    <row r="18" spans="6:7" s="47" customFormat="1"/>
-    <row r="19" spans="6:7" s="47" customFormat="1"/>
-    <row r="20" spans="6:7" s="47" customFormat="1"/>
-    <row r="21" spans="6:7" s="47" customFormat="1"/>
-    <row r="22" spans="6:7" s="47" customFormat="1"/>
-    <row r="23" spans="6:7" s="47" customFormat="1"/>
-    <row r="24" spans="6:7" s="47" customFormat="1"/>
-    <row r="25" spans="6:7" s="47" customFormat="1">
+      <c r="H16" s="45"/>
+    </row>
+    <row r="17" spans="6:8" s="47" customFormat="1">
+      <c r="H17" s="45"/>
+    </row>
+    <row r="18" spans="6:8" s="47" customFormat="1">
+      <c r="H18" s="45"/>
+    </row>
+    <row r="19" spans="6:8" s="47" customFormat="1">
+      <c r="H19" s="45"/>
+    </row>
+    <row r="20" spans="6:8" s="47" customFormat="1">
+      <c r="H20" s="45"/>
+    </row>
+    <row r="21" spans="6:8" s="47" customFormat="1">
+      <c r="H21" s="45"/>
+    </row>
+    <row r="22" spans="6:8" s="47" customFormat="1">
+      <c r="H22" s="45"/>
+    </row>
+    <row r="23" spans="6:8" s="47" customFormat="1">
+      <c r="H23" s="45"/>
+    </row>
+    <row r="24" spans="6:8" s="47" customFormat="1">
+      <c r="H24" s="45"/>
+    </row>
+    <row r="25" spans="6:8" s="47" customFormat="1">
       <c r="F25" s="49"/>
       <c r="G25" s="50"/>
-    </row>
-    <row r="26" spans="6:7" s="47" customFormat="1"/>
-    <row r="27" spans="6:7" s="47" customFormat="1"/>
-    <row r="28" spans="6:7" s="47" customFormat="1"/>
-    <row r="29" spans="6:7" s="47" customFormat="1"/>
-    <row r="30" spans="6:7" s="47" customFormat="1"/>
-    <row r="31" spans="6:7" s="47" customFormat="1">
+      <c r="H25" s="45"/>
+    </row>
+    <row r="26" spans="6:8" s="47" customFormat="1">
+      <c r="H26" s="45"/>
+    </row>
+    <row r="27" spans="6:8" s="47" customFormat="1">
+      <c r="H27" s="45"/>
+    </row>
+    <row r="28" spans="6:8" s="47" customFormat="1">
+      <c r="H28" s="45"/>
+    </row>
+    <row r="29" spans="6:8" s="47" customFormat="1">
+      <c r="H29" s="45"/>
+    </row>
+    <row r="30" spans="6:8" s="47" customFormat="1">
+      <c r="H30" s="45"/>
+    </row>
+    <row r="31" spans="6:8" s="47" customFormat="1">
       <c r="F31" s="49"/>
       <c r="G31" s="50"/>
-    </row>
-    <row r="32" spans="6:7" s="47" customFormat="1"/>
-    <row r="33" s="47" customFormat="1"/>
-    <row r="34" s="47" customFormat="1"/>
-    <row r="35" s="47" customFormat="1"/>
-    <row r="36" s="47" customFormat="1"/>
-    <row r="37" s="47" customFormat="1"/>
-    <row r="38" s="47" customFormat="1"/>
-    <row r="39" s="47" customFormat="1"/>
-    <row r="40" s="47" customFormat="1"/>
-    <row r="41" s="47" customFormat="1"/>
-    <row r="42" s="47" customFormat="1"/>
-    <row r="43" s="47" customFormat="1"/>
-    <row r="44" s="47" customFormat="1"/>
-    <row r="45" s="47" customFormat="1"/>
-    <row r="46" s="47" customFormat="1"/>
-    <row r="47" s="47" customFormat="1"/>
-    <row r="48" s="47" customFormat="1"/>
-    <row r="49" s="47" customFormat="1"/>
-    <row r="50" s="47" customFormat="1"/>
-    <row r="51" s="47" customFormat="1"/>
-    <row r="52" s="47" customFormat="1"/>
-    <row r="53" s="47" customFormat="1"/>
-    <row r="54" s="47" customFormat="1"/>
-    <row r="55" s="47" customFormat="1"/>
-    <row r="56" s="47" customFormat="1"/>
-    <row r="57" s="47" customFormat="1"/>
-    <row r="58" s="47" customFormat="1"/>
-    <row r="59" s="47" customFormat="1"/>
-    <row r="60" s="47" customFormat="1"/>
-    <row r="61" s="47" customFormat="1"/>
-    <row r="62" s="47" customFormat="1"/>
-    <row r="63" s="47" customFormat="1"/>
-    <row r="64" s="47" customFormat="1"/>
-    <row r="65" s="47" customFormat="1"/>
-    <row r="66" s="47" customFormat="1"/>
-    <row r="67" s="47" customFormat="1"/>
-    <row r="68" s="47" customFormat="1"/>
-    <row r="69" s="47" customFormat="1"/>
-    <row r="70" s="47" customFormat="1"/>
-    <row r="71" s="47" customFormat="1"/>
-    <row r="72" s="47" customFormat="1"/>
-    <row r="73" s="47" customFormat="1"/>
-    <row r="74" s="47" customFormat="1"/>
-    <row r="75" s="47" customFormat="1"/>
-    <row r="76" s="47" customFormat="1"/>
-    <row r="77" s="47" customFormat="1"/>
-    <row r="78" s="47" customFormat="1"/>
-    <row r="79" s="47" customFormat="1"/>
-    <row r="80" s="47" customFormat="1"/>
-    <row r="81" s="47" customFormat="1"/>
-    <row r="82" s="47" customFormat="1"/>
-    <row r="83" s="47" customFormat="1"/>
-    <row r="84" s="47" customFormat="1"/>
-    <row r="85" s="47" customFormat="1"/>
-    <row r="86" s="47" customFormat="1"/>
-    <row r="87" s="47" customFormat="1"/>
-    <row r="88" s="47" customFormat="1"/>
-    <row r="89" s="47" customFormat="1"/>
-    <row r="90" s="47" customFormat="1"/>
-    <row r="91" s="47" customFormat="1"/>
-    <row r="92" s="47" customFormat="1"/>
-    <row r="93" s="47" customFormat="1"/>
-    <row r="94" s="47" customFormat="1"/>
-    <row r="95" s="47" customFormat="1"/>
-    <row r="96" s="47" customFormat="1"/>
-    <row r="97" s="47" customFormat="1"/>
-    <row r="98" s="47" customFormat="1"/>
-    <row r="99" s="47" customFormat="1"/>
-    <row r="100" s="47" customFormat="1"/>
-    <row r="101" s="47" customFormat="1"/>
-    <row r="102" s="47" customFormat="1"/>
-    <row r="103" s="47" customFormat="1"/>
-    <row r="104" s="47" customFormat="1"/>
-    <row r="105" s="47" customFormat="1"/>
-    <row r="106" s="47" customFormat="1"/>
-    <row r="107" s="47" customFormat="1"/>
-    <row r="108" s="47" customFormat="1"/>
-    <row r="109" s="47" customFormat="1"/>
-    <row r="110" s="47" customFormat="1"/>
-    <row r="111" s="47" customFormat="1"/>
-    <row r="112" s="47" customFormat="1"/>
-    <row r="113" s="47" customFormat="1"/>
-    <row r="114" s="47" customFormat="1"/>
-    <row r="115" s="47" customFormat="1"/>
-    <row r="116" s="47" customFormat="1"/>
-    <row r="117" s="47" customFormat="1"/>
-    <row r="118" s="47" customFormat="1"/>
-    <row r="119" s="47" customFormat="1"/>
-    <row r="120" s="47" customFormat="1"/>
-    <row r="121" s="47" customFormat="1"/>
-    <row r="122" s="47" customFormat="1"/>
-    <row r="123" s="47" customFormat="1"/>
-    <row r="124" s="47" customFormat="1"/>
-    <row r="125" s="47" customFormat="1"/>
-    <row r="126" s="47" customFormat="1"/>
-    <row r="127" s="47" customFormat="1"/>
-    <row r="128" s="47" customFormat="1"/>
-    <row r="129" s="47" customFormat="1"/>
-    <row r="130" s="47" customFormat="1"/>
-    <row r="131" s="47" customFormat="1"/>
-    <row r="132" s="47" customFormat="1"/>
-    <row r="133" s="47" customFormat="1"/>
-    <row r="134" s="47" customFormat="1"/>
-    <row r="135" s="47" customFormat="1"/>
-    <row r="136" s="47" customFormat="1"/>
-    <row r="137" s="47" customFormat="1"/>
-    <row r="138" s="47" customFormat="1"/>
-    <row r="139" s="47" customFormat="1"/>
-    <row r="140" s="47" customFormat="1"/>
-    <row r="141" s="47" customFormat="1"/>
-    <row r="142" s="47" customFormat="1"/>
-    <row r="143" s="47" customFormat="1"/>
-    <row r="144" s="47" customFormat="1"/>
-    <row r="145" s="47" customFormat="1"/>
-    <row r="146" s="47" customFormat="1"/>
-    <row r="147" s="47" customFormat="1"/>
-    <row r="148" s="47" customFormat="1"/>
-    <row r="149" s="47" customFormat="1"/>
-    <row r="150" s="47" customFormat="1"/>
-    <row r="151" s="47" customFormat="1"/>
-    <row r="152" s="47" customFormat="1"/>
-    <row r="153" s="47" customFormat="1"/>
-    <row r="154" s="47" customFormat="1"/>
-    <row r="155" s="47" customFormat="1"/>
-    <row r="156" s="47" customFormat="1"/>
-    <row r="157" s="47" customFormat="1"/>
-    <row r="158" s="47" customFormat="1"/>
-    <row r="159" s="47" customFormat="1"/>
-    <row r="160" s="47" customFormat="1"/>
-    <row r="161" s="47" customFormat="1"/>
-    <row r="162" s="47" customFormat="1"/>
-    <row r="163" s="47" customFormat="1"/>
-    <row r="164" s="47" customFormat="1"/>
-    <row r="165" s="47" customFormat="1"/>
-    <row r="166" s="47" customFormat="1"/>
-    <row r="167" s="47" customFormat="1"/>
-    <row r="168" s="47" customFormat="1"/>
-    <row r="169" s="47" customFormat="1"/>
-    <row r="170" s="47" customFormat="1"/>
-    <row r="171" s="47" customFormat="1"/>
-    <row r="172" s="47" customFormat="1"/>
-    <row r="173" s="47" customFormat="1"/>
-    <row r="174" s="47" customFormat="1"/>
-    <row r="175" s="47" customFormat="1"/>
-    <row r="176" s="47" customFormat="1"/>
-    <row r="177" s="47" customFormat="1"/>
-    <row r="178" s="47" customFormat="1"/>
-    <row r="179" s="47" customFormat="1"/>
-    <row r="180" s="47" customFormat="1"/>
-    <row r="181" s="47" customFormat="1"/>
-    <row r="182" s="47" customFormat="1"/>
-    <row r="183" s="47" customFormat="1"/>
-    <row r="184" s="47" customFormat="1"/>
-    <row r="185" s="47" customFormat="1"/>
-    <row r="186" s="47" customFormat="1"/>
-    <row r="187" s="47" customFormat="1"/>
-    <row r="188" s="47" customFormat="1"/>
-    <row r="189" s="47" customFormat="1"/>
-    <row r="190" s="47" customFormat="1"/>
-    <row r="191" s="47" customFormat="1"/>
-    <row r="192" s="47" customFormat="1"/>
-    <row r="193" s="47" customFormat="1"/>
-    <row r="194" s="47" customFormat="1"/>
-    <row r="195" s="47" customFormat="1"/>
-    <row r="196" s="47" customFormat="1"/>
-    <row r="197" s="47" customFormat="1"/>
-    <row r="198" s="47" customFormat="1"/>
-    <row r="199" s="47" customFormat="1"/>
-    <row r="200" s="47" customFormat="1"/>
-    <row r="201" s="47" customFormat="1"/>
-    <row r="202" s="47" customFormat="1"/>
-    <row r="203" s="47" customFormat="1"/>
-    <row r="204" s="47" customFormat="1"/>
-    <row r="205" s="47" customFormat="1"/>
-    <row r="206" s="47" customFormat="1"/>
-    <row r="207" s="47" customFormat="1"/>
-    <row r="208" s="47" customFormat="1"/>
-    <row r="209" s="47" customFormat="1"/>
-    <row r="210" s="47" customFormat="1"/>
-    <row r="211" s="47" customFormat="1"/>
-    <row r="212" s="47" customFormat="1"/>
-    <row r="213" s="47" customFormat="1"/>
-    <row r="214" s="47" customFormat="1"/>
-    <row r="215" s="47" customFormat="1"/>
-    <row r="216" s="47" customFormat="1"/>
-    <row r="217" s="47" customFormat="1"/>
-    <row r="218" s="47" customFormat="1"/>
-    <row r="219" s="47" customFormat="1"/>
-    <row r="220" s="47" customFormat="1"/>
-    <row r="221" s="47" customFormat="1"/>
-    <row r="222" s="47" customFormat="1"/>
-    <row r="223" s="47" customFormat="1"/>
-    <row r="224" s="47" customFormat="1"/>
-    <row r="225" s="47" customFormat="1"/>
-    <row r="226" s="47" customFormat="1"/>
-    <row r="227" s="47" customFormat="1"/>
-    <row r="228" s="47" customFormat="1"/>
-    <row r="229" s="47" customFormat="1"/>
-    <row r="230" s="47" customFormat="1"/>
-    <row r="231" s="47" customFormat="1"/>
-    <row r="232" s="47" customFormat="1"/>
-    <row r="233" s="47" customFormat="1"/>
-    <row r="234" s="47" customFormat="1"/>
-    <row r="235" s="47" customFormat="1"/>
-    <row r="236" s="47" customFormat="1"/>
-    <row r="237" s="47" customFormat="1"/>
-    <row r="238" s="47" customFormat="1"/>
-    <row r="239" s="47" customFormat="1"/>
-    <row r="240" s="47" customFormat="1"/>
-    <row r="241" s="47" customFormat="1"/>
-    <row r="242" s="47" customFormat="1"/>
-    <row r="243" s="47" customFormat="1"/>
-    <row r="244" s="47" customFormat="1"/>
-    <row r="245" s="47" customFormat="1"/>
-    <row r="246" s="47" customFormat="1"/>
-    <row r="247" s="47" customFormat="1"/>
-    <row r="248" s="47" customFormat="1"/>
-    <row r="249" s="47" customFormat="1"/>
-    <row r="250" s="47" customFormat="1"/>
-    <row r="251" s="47" customFormat="1"/>
-    <row r="252" s="47" customFormat="1"/>
-    <row r="253" s="47" customFormat="1"/>
-    <row r="254" s="47" customFormat="1"/>
-    <row r="255" s="47" customFormat="1"/>
-    <row r="256" s="47" customFormat="1"/>
-    <row r="257" s="47" customFormat="1"/>
-    <row r="258" s="47" customFormat="1"/>
-    <row r="259" s="47" customFormat="1"/>
-    <row r="260" s="47" customFormat="1"/>
-    <row r="261" s="47" customFormat="1"/>
-    <row r="262" s="47" customFormat="1"/>
-    <row r="263" s="47" customFormat="1"/>
-    <row r="264" s="47" customFormat="1"/>
-    <row r="265" s="47" customFormat="1"/>
-    <row r="266" s="47" customFormat="1"/>
-    <row r="267" s="47" customFormat="1"/>
-    <row r="268" s="47" customFormat="1"/>
-    <row r="269" s="47" customFormat="1"/>
-    <row r="270" s="47" customFormat="1"/>
-    <row r="271" s="47" customFormat="1"/>
-    <row r="272" s="47" customFormat="1"/>
-    <row r="273" s="47" customFormat="1"/>
-    <row r="274" s="47" customFormat="1"/>
-    <row r="275" s="47" customFormat="1"/>
-    <row r="276" s="47" customFormat="1"/>
-    <row r="277" s="47" customFormat="1"/>
-    <row r="278" s="47" customFormat="1"/>
-    <row r="279" s="47" customFormat="1"/>
-    <row r="280" s="47" customFormat="1"/>
-    <row r="281" s="47" customFormat="1"/>
-    <row r="282" s="47" customFormat="1"/>
-    <row r="283" s="47" customFormat="1"/>
-    <row r="284" s="47" customFormat="1"/>
-    <row r="285" s="47" customFormat="1"/>
-    <row r="286" s="47" customFormat="1"/>
-    <row r="287" s="47" customFormat="1"/>
-    <row r="288" s="47" customFormat="1"/>
-    <row r="289" s="47" customFormat="1"/>
-    <row r="290" s="47" customFormat="1"/>
-    <row r="291" s="47" customFormat="1"/>
-    <row r="292" s="47" customFormat="1"/>
-    <row r="293" s="47" customFormat="1"/>
-    <row r="294" s="47" customFormat="1"/>
-    <row r="295" s="47" customFormat="1"/>
-    <row r="296" s="47" customFormat="1"/>
-    <row r="297" s="47" customFormat="1"/>
-    <row r="298" s="47" customFormat="1"/>
-    <row r="299" s="47" customFormat="1"/>
-    <row r="300" s="47" customFormat="1"/>
-    <row r="301" s="47" customFormat="1"/>
-    <row r="302" s="47" customFormat="1"/>
-    <row r="303" s="47" customFormat="1"/>
-    <row r="304" s="47" customFormat="1"/>
-    <row r="305" s="47" customFormat="1"/>
-    <row r="306" s="47" customFormat="1"/>
-    <row r="307" s="47" customFormat="1"/>
-    <row r="308" s="47" customFormat="1"/>
-    <row r="309" s="47" customFormat="1"/>
-    <row r="310" s="47" customFormat="1"/>
-    <row r="311" s="47" customFormat="1"/>
-    <row r="312" s="47" customFormat="1"/>
-    <row r="313" s="47" customFormat="1"/>
-    <row r="314" s="47" customFormat="1"/>
-    <row r="315" s="47" customFormat="1"/>
-    <row r="316" s="47" customFormat="1"/>
-    <row r="317" s="47" customFormat="1"/>
-    <row r="318" s="47" customFormat="1"/>
-    <row r="319" s="47" customFormat="1"/>
-    <row r="320" s="47" customFormat="1"/>
-    <row r="321" s="47" customFormat="1"/>
-    <row r="322" s="47" customFormat="1"/>
-    <row r="323" s="47" customFormat="1"/>
-    <row r="324" s="47" customFormat="1"/>
-    <row r="325" s="47" customFormat="1"/>
-    <row r="326" s="47" customFormat="1"/>
-    <row r="327" s="47" customFormat="1"/>
-    <row r="328" s="47" customFormat="1"/>
-    <row r="329" s="47" customFormat="1"/>
-    <row r="330" s="47" customFormat="1"/>
-    <row r="331" s="47" customFormat="1"/>
-    <row r="332" s="47" customFormat="1"/>
-    <row r="333" s="47" customFormat="1"/>
-    <row r="334" s="47" customFormat="1"/>
+      <c r="H31" s="45"/>
+    </row>
+    <row r="32" spans="6:8" s="47" customFormat="1">
+      <c r="H32" s="45"/>
+    </row>
+    <row r="33" spans="8:8" s="47" customFormat="1">
+      <c r="H33" s="45"/>
+    </row>
+    <row r="34" spans="8:8" s="47" customFormat="1">
+      <c r="H34" s="45"/>
+    </row>
+    <row r="35" spans="8:8" s="47" customFormat="1">
+      <c r="H35" s="45"/>
+    </row>
+    <row r="36" spans="8:8" s="47" customFormat="1">
+      <c r="H36" s="45"/>
+    </row>
+    <row r="37" spans="8:8" s="47" customFormat="1">
+      <c r="H37" s="45"/>
+    </row>
+    <row r="38" spans="8:8" s="47" customFormat="1">
+      <c r="H38" s="45"/>
+    </row>
+    <row r="39" spans="8:8" s="47" customFormat="1">
+      <c r="H39" s="45"/>
+    </row>
+    <row r="40" spans="8:8" s="47" customFormat="1">
+      <c r="H40" s="45"/>
+    </row>
+    <row r="41" spans="8:8" s="47" customFormat="1">
+      <c r="H41" s="45"/>
+    </row>
+    <row r="42" spans="8:8" s="47" customFormat="1">
+      <c r="H42" s="45"/>
+    </row>
+    <row r="43" spans="8:8" s="47" customFormat="1">
+      <c r="H43" s="45"/>
+    </row>
+    <row r="44" spans="8:8" s="47" customFormat="1">
+      <c r="H44" s="45"/>
+    </row>
+    <row r="45" spans="8:8" s="47" customFormat="1">
+      <c r="H45" s="45"/>
+    </row>
+    <row r="46" spans="8:8" s="47" customFormat="1">
+      <c r="H46" s="45"/>
+    </row>
+    <row r="47" spans="8:8" s="47" customFormat="1">
+      <c r="H47" s="45"/>
+    </row>
+    <row r="48" spans="8:8" s="47" customFormat="1">
+      <c r="H48" s="45"/>
+    </row>
+    <row r="49" spans="8:8" s="47" customFormat="1">
+      <c r="H49" s="45"/>
+    </row>
+    <row r="50" spans="8:8" s="47" customFormat="1">
+      <c r="H50" s="45"/>
+    </row>
+    <row r="51" spans="8:8" s="47" customFormat="1">
+      <c r="H51" s="45"/>
+    </row>
+    <row r="52" spans="8:8" s="47" customFormat="1">
+      <c r="H52" s="45"/>
+    </row>
+    <row r="53" spans="8:8" s="47" customFormat="1">
+      <c r="H53" s="45"/>
+    </row>
+    <row r="54" spans="8:8" s="47" customFormat="1">
+      <c r="H54" s="45"/>
+    </row>
+    <row r="55" spans="8:8" s="47" customFormat="1">
+      <c r="H55" s="45"/>
+    </row>
+    <row r="56" spans="8:8" s="47" customFormat="1">
+      <c r="H56" s="45"/>
+    </row>
+    <row r="57" spans="8:8" s="47" customFormat="1">
+      <c r="H57" s="45"/>
+    </row>
+    <row r="58" spans="8:8" s="47" customFormat="1">
+      <c r="H58" s="45"/>
+    </row>
+    <row r="59" spans="8:8" s="47" customFormat="1">
+      <c r="H59" s="45"/>
+    </row>
+    <row r="60" spans="8:8" s="47" customFormat="1">
+      <c r="H60" s="45"/>
+    </row>
+    <row r="61" spans="8:8" s="47" customFormat="1">
+      <c r="H61" s="45"/>
+    </row>
+    <row r="62" spans="8:8" s="47" customFormat="1">
+      <c r="H62" s="45"/>
+    </row>
+    <row r="63" spans="8:8" s="47" customFormat="1">
+      <c r="H63" s="45"/>
+    </row>
+    <row r="64" spans="8:8" s="47" customFormat="1">
+      <c r="H64" s="45"/>
+    </row>
+    <row r="65" spans="8:8" s="47" customFormat="1">
+      <c r="H65" s="45"/>
+    </row>
+    <row r="66" spans="8:8" s="47" customFormat="1">
+      <c r="H66" s="45"/>
+    </row>
+    <row r="67" spans="8:8" s="47" customFormat="1">
+      <c r="H67" s="45"/>
+    </row>
+    <row r="68" spans="8:8" s="47" customFormat="1">
+      <c r="H68" s="45"/>
+    </row>
+    <row r="69" spans="8:8" s="47" customFormat="1">
+      <c r="H69" s="45"/>
+    </row>
+    <row r="70" spans="8:8" s="47" customFormat="1">
+      <c r="H70" s="45"/>
+    </row>
+    <row r="71" spans="8:8" s="47" customFormat="1">
+      <c r="H71" s="45"/>
+    </row>
+    <row r="72" spans="8:8" s="47" customFormat="1">
+      <c r="H72" s="45"/>
+    </row>
+    <row r="73" spans="8:8" s="47" customFormat="1">
+      <c r="H73" s="45"/>
+    </row>
+    <row r="74" spans="8:8" s="47" customFormat="1">
+      <c r="H74" s="45"/>
+    </row>
+    <row r="75" spans="8:8" s="47" customFormat="1">
+      <c r="H75" s="45"/>
+    </row>
+    <row r="76" spans="8:8" s="47" customFormat="1">
+      <c r="H76" s="45"/>
+    </row>
+    <row r="77" spans="8:8" s="47" customFormat="1">
+      <c r="H77" s="45"/>
+    </row>
+    <row r="78" spans="8:8" s="47" customFormat="1">
+      <c r="H78" s="45"/>
+    </row>
+    <row r="79" spans="8:8" s="47" customFormat="1">
+      <c r="H79" s="45"/>
+    </row>
+    <row r="80" spans="8:8" s="47" customFormat="1">
+      <c r="H80" s="45"/>
+    </row>
+    <row r="81" spans="8:8" s="47" customFormat="1">
+      <c r="H81" s="45"/>
+    </row>
+    <row r="82" spans="8:8" s="47" customFormat="1">
+      <c r="H82" s="45"/>
+    </row>
+    <row r="83" spans="8:8" s="47" customFormat="1">
+      <c r="H83" s="45"/>
+    </row>
+    <row r="84" spans="8:8" s="47" customFormat="1">
+      <c r="H84" s="45"/>
+    </row>
+    <row r="85" spans="8:8" s="47" customFormat="1">
+      <c r="H85" s="45"/>
+    </row>
+    <row r="86" spans="8:8" s="47" customFormat="1">
+      <c r="H86" s="45"/>
+    </row>
+    <row r="87" spans="8:8" s="47" customFormat="1">
+      <c r="H87" s="45"/>
+    </row>
+    <row r="88" spans="8:8" s="47" customFormat="1">
+      <c r="H88" s="45"/>
+    </row>
+    <row r="89" spans="8:8" s="47" customFormat="1">
+      <c r="H89" s="45"/>
+    </row>
+    <row r="90" spans="8:8" s="47" customFormat="1">
+      <c r="H90" s="45"/>
+    </row>
+    <row r="91" spans="8:8" s="47" customFormat="1">
+      <c r="H91" s="45"/>
+    </row>
+    <row r="92" spans="8:8" s="47" customFormat="1">
+      <c r="H92" s="45"/>
+    </row>
+    <row r="93" spans="8:8" s="47" customFormat="1">
+      <c r="H93" s="45"/>
+    </row>
+    <row r="94" spans="8:8" s="47" customFormat="1">
+      <c r="H94" s="45"/>
+    </row>
+    <row r="95" spans="8:8" s="47" customFormat="1">
+      <c r="H95" s="45"/>
+    </row>
+    <row r="96" spans="8:8" s="47" customFormat="1">
+      <c r="H96" s="45"/>
+    </row>
+    <row r="97" spans="8:8" s="47" customFormat="1">
+      <c r="H97" s="45"/>
+    </row>
+    <row r="98" spans="8:8" s="47" customFormat="1">
+      <c r="H98" s="45"/>
+    </row>
+    <row r="99" spans="8:8" s="47" customFormat="1">
+      <c r="H99" s="45"/>
+    </row>
+    <row r="100" spans="8:8" s="47" customFormat="1">
+      <c r="H100" s="45"/>
+    </row>
+    <row r="101" spans="8:8" s="47" customFormat="1">
+      <c r="H101" s="45"/>
+    </row>
+    <row r="102" spans="8:8" s="47" customFormat="1">
+      <c r="H102" s="45"/>
+    </row>
+    <row r="103" spans="8:8" s="47" customFormat="1">
+      <c r="H103" s="45"/>
+    </row>
+    <row r="104" spans="8:8" s="47" customFormat="1">
+      <c r="H104" s="45"/>
+    </row>
+    <row r="105" spans="8:8" s="47" customFormat="1">
+      <c r="H105" s="45"/>
+    </row>
+    <row r="106" spans="8:8" s="47" customFormat="1">
+      <c r="H106" s="45"/>
+    </row>
+    <row r="107" spans="8:8" s="47" customFormat="1">
+      <c r="H107" s="45"/>
+    </row>
+    <row r="108" spans="8:8" s="47" customFormat="1">
+      <c r="H108" s="45"/>
+    </row>
+    <row r="109" spans="8:8" s="47" customFormat="1">
+      <c r="H109" s="45"/>
+    </row>
+    <row r="110" spans="8:8" s="47" customFormat="1">
+      <c r="H110" s="45"/>
+    </row>
+    <row r="111" spans="8:8" s="47" customFormat="1">
+      <c r="H111" s="45"/>
+    </row>
+    <row r="112" spans="8:8" s="47" customFormat="1">
+      <c r="H112" s="45"/>
+    </row>
+    <row r="113" spans="8:8" s="47" customFormat="1">
+      <c r="H113" s="45"/>
+    </row>
+    <row r="114" spans="8:8" s="47" customFormat="1">
+      <c r="H114" s="45"/>
+    </row>
+    <row r="115" spans="8:8" s="47" customFormat="1">
+      <c r="H115" s="45"/>
+    </row>
+    <row r="116" spans="8:8" s="47" customFormat="1">
+      <c r="H116" s="45"/>
+    </row>
+    <row r="117" spans="8:8" s="47" customFormat="1">
+      <c r="H117" s="45"/>
+    </row>
+    <row r="118" spans="8:8" s="47" customFormat="1">
+      <c r="H118" s="45"/>
+    </row>
+    <row r="119" spans="8:8" s="47" customFormat="1">
+      <c r="H119" s="45"/>
+    </row>
+    <row r="120" spans="8:8" s="47" customFormat="1">
+      <c r="H120" s="45"/>
+    </row>
+    <row r="121" spans="8:8" s="47" customFormat="1">
+      <c r="H121" s="45"/>
+    </row>
+    <row r="122" spans="8:8" s="47" customFormat="1">
+      <c r="H122" s="45"/>
+    </row>
+    <row r="123" spans="8:8" s="47" customFormat="1">
+      <c r="H123" s="45"/>
+    </row>
+    <row r="124" spans="8:8" s="47" customFormat="1">
+      <c r="H124" s="45"/>
+    </row>
+    <row r="125" spans="8:8" s="47" customFormat="1">
+      <c r="H125" s="45"/>
+    </row>
+    <row r="126" spans="8:8" s="47" customFormat="1">
+      <c r="H126" s="45"/>
+    </row>
+    <row r="127" spans="8:8" s="47" customFormat="1">
+      <c r="H127" s="45"/>
+    </row>
+    <row r="128" spans="8:8" s="47" customFormat="1">
+      <c r="H128" s="45"/>
+    </row>
+    <row r="129" spans="8:8" s="47" customFormat="1">
+      <c r="H129" s="45"/>
+    </row>
+    <row r="130" spans="8:8" s="47" customFormat="1">
+      <c r="H130" s="45"/>
+    </row>
+    <row r="131" spans="8:8" s="47" customFormat="1">
+      <c r="H131" s="45"/>
+    </row>
+    <row r="132" spans="8:8" s="47" customFormat="1">
+      <c r="H132" s="45"/>
+    </row>
+    <row r="133" spans="8:8" s="47" customFormat="1">
+      <c r="H133" s="45"/>
+    </row>
+    <row r="134" spans="8:8" s="47" customFormat="1">
+      <c r="H134" s="45"/>
+    </row>
+    <row r="135" spans="8:8" s="47" customFormat="1">
+      <c r="H135" s="45"/>
+    </row>
+    <row r="136" spans="8:8" s="47" customFormat="1">
+      <c r="H136" s="45"/>
+    </row>
+    <row r="137" spans="8:8" s="47" customFormat="1">
+      <c r="H137" s="45"/>
+    </row>
+    <row r="138" spans="8:8" s="47" customFormat="1">
+      <c r="H138" s="45"/>
+    </row>
+    <row r="139" spans="8:8" s="47" customFormat="1">
+      <c r="H139" s="45"/>
+    </row>
+    <row r="140" spans="8:8" s="47" customFormat="1">
+      <c r="H140" s="45"/>
+    </row>
+    <row r="141" spans="8:8" s="47" customFormat="1">
+      <c r="H141" s="45"/>
+    </row>
+    <row r="142" spans="8:8" s="47" customFormat="1">
+      <c r="H142" s="45"/>
+    </row>
+    <row r="143" spans="8:8" s="47" customFormat="1">
+      <c r="H143" s="45"/>
+    </row>
+    <row r="144" spans="8:8" s="47" customFormat="1">
+      <c r="H144" s="45"/>
+    </row>
+    <row r="145" spans="8:8" s="47" customFormat="1">
+      <c r="H145" s="45"/>
+    </row>
+    <row r="146" spans="8:8" s="47" customFormat="1">
+      <c r="H146" s="45"/>
+    </row>
+    <row r="147" spans="8:8" s="47" customFormat="1">
+      <c r="H147" s="45"/>
+    </row>
+    <row r="148" spans="8:8" s="47" customFormat="1">
+      <c r="H148" s="45"/>
+    </row>
+    <row r="149" spans="8:8" s="47" customFormat="1">
+      <c r="H149" s="45"/>
+    </row>
+    <row r="150" spans="8:8" s="47" customFormat="1">
+      <c r="H150" s="45"/>
+    </row>
+    <row r="151" spans="8:8" s="47" customFormat="1">
+      <c r="H151" s="45"/>
+    </row>
+    <row r="152" spans="8:8" s="47" customFormat="1">
+      <c r="H152" s="45"/>
+    </row>
+    <row r="153" spans="8:8" s="47" customFormat="1">
+      <c r="H153" s="45"/>
+    </row>
+    <row r="154" spans="8:8" s="47" customFormat="1">
+      <c r="H154" s="45"/>
+    </row>
+    <row r="155" spans="8:8" s="47" customFormat="1">
+      <c r="H155" s="45"/>
+    </row>
+    <row r="156" spans="8:8" s="47" customFormat="1">
+      <c r="H156" s="45"/>
+    </row>
+    <row r="157" spans="8:8" s="47" customFormat="1">
+      <c r="H157" s="45"/>
+    </row>
+    <row r="158" spans="8:8" s="47" customFormat="1">
+      <c r="H158" s="45"/>
+    </row>
+    <row r="159" spans="8:8" s="47" customFormat="1">
+      <c r="H159" s="45"/>
+    </row>
+    <row r="160" spans="8:8" s="47" customFormat="1">
+      <c r="H160" s="45"/>
+    </row>
+    <row r="161" spans="8:8" s="47" customFormat="1">
+      <c r="H161" s="45"/>
+    </row>
+    <row r="162" spans="8:8" s="47" customFormat="1">
+      <c r="H162" s="45"/>
+    </row>
+    <row r="163" spans="8:8" s="47" customFormat="1">
+      <c r="H163" s="45"/>
+    </row>
+    <row r="164" spans="8:8" s="47" customFormat="1">
+      <c r="H164" s="45"/>
+    </row>
+    <row r="165" spans="8:8" s="47" customFormat="1">
+      <c r="H165" s="45"/>
+    </row>
+    <row r="166" spans="8:8" s="47" customFormat="1">
+      <c r="H166" s="45"/>
+    </row>
+    <row r="167" spans="8:8" s="47" customFormat="1">
+      <c r="H167" s="45"/>
+    </row>
+    <row r="168" spans="8:8" s="47" customFormat="1">
+      <c r="H168" s="45"/>
+    </row>
+    <row r="169" spans="8:8" s="47" customFormat="1">
+      <c r="H169" s="45"/>
+    </row>
+    <row r="170" spans="8:8" s="47" customFormat="1">
+      <c r="H170" s="45"/>
+    </row>
+    <row r="171" spans="8:8" s="47" customFormat="1">
+      <c r="H171" s="45"/>
+    </row>
+    <row r="172" spans="8:8" s="47" customFormat="1">
+      <c r="H172" s="45"/>
+    </row>
+    <row r="173" spans="8:8" s="47" customFormat="1">
+      <c r="H173" s="45"/>
+    </row>
+    <row r="174" spans="8:8" s="47" customFormat="1">
+      <c r="H174" s="45"/>
+    </row>
+    <row r="175" spans="8:8" s="47" customFormat="1">
+      <c r="H175" s="45"/>
+    </row>
+    <row r="176" spans="8:8" s="47" customFormat="1">
+      <c r="H176" s="45"/>
+    </row>
+    <row r="177" spans="8:8" s="47" customFormat="1">
+      <c r="H177" s="45"/>
+    </row>
+    <row r="178" spans="8:8" s="47" customFormat="1">
+      <c r="H178" s="45"/>
+    </row>
+    <row r="179" spans="8:8" s="47" customFormat="1">
+      <c r="H179" s="45"/>
+    </row>
+    <row r="180" spans="8:8" s="47" customFormat="1">
+      <c r="H180" s="45"/>
+    </row>
+    <row r="181" spans="8:8" s="47" customFormat="1">
+      <c r="H181" s="45"/>
+    </row>
+    <row r="182" spans="8:8" s="47" customFormat="1">
+      <c r="H182" s="45"/>
+    </row>
+    <row r="183" spans="8:8" s="47" customFormat="1">
+      <c r="H183" s="45"/>
+    </row>
+    <row r="184" spans="8:8" s="47" customFormat="1">
+      <c r="H184" s="45"/>
+    </row>
+    <row r="185" spans="8:8" s="47" customFormat="1">
+      <c r="H185" s="45"/>
+    </row>
+    <row r="186" spans="8:8" s="47" customFormat="1">
+      <c r="H186" s="45"/>
+    </row>
+    <row r="187" spans="8:8" s="47" customFormat="1">
+      <c r="H187" s="45"/>
+    </row>
+    <row r="188" spans="8:8" s="47" customFormat="1">
+      <c r="H188" s="45"/>
+    </row>
+    <row r="189" spans="8:8" s="47" customFormat="1">
+      <c r="H189" s="45"/>
+    </row>
+    <row r="190" spans="8:8" s="47" customFormat="1">
+      <c r="H190" s="45"/>
+    </row>
+    <row r="191" spans="8:8" s="47" customFormat="1">
+      <c r="H191" s="45"/>
+    </row>
+    <row r="192" spans="8:8" s="47" customFormat="1">
+      <c r="H192" s="45"/>
+    </row>
+    <row r="193" spans="8:8" s="47" customFormat="1">
+      <c r="H193" s="45"/>
+    </row>
+    <row r="194" spans="8:8" s="47" customFormat="1">
+      <c r="H194" s="45"/>
+    </row>
+    <row r="195" spans="8:8" s="47" customFormat="1">
+      <c r="H195" s="45"/>
+    </row>
+    <row r="196" spans="8:8" s="47" customFormat="1">
+      <c r="H196" s="45"/>
+    </row>
+    <row r="197" spans="8:8" s="47" customFormat="1">
+      <c r="H197" s="45"/>
+    </row>
+    <row r="198" spans="8:8" s="47" customFormat="1">
+      <c r="H198" s="45"/>
+    </row>
+    <row r="199" spans="8:8" s="47" customFormat="1">
+      <c r="H199" s="45"/>
+    </row>
+    <row r="200" spans="8:8" s="47" customFormat="1">
+      <c r="H200" s="45"/>
+    </row>
+    <row r="201" spans="8:8" s="47" customFormat="1">
+      <c r="H201" s="45"/>
+    </row>
+    <row r="202" spans="8:8" s="47" customFormat="1">
+      <c r="H202" s="45"/>
+    </row>
+    <row r="203" spans="8:8" s="47" customFormat="1">
+      <c r="H203" s="45"/>
+    </row>
+    <row r="204" spans="8:8" s="47" customFormat="1">
+      <c r="H204" s="45"/>
+    </row>
+    <row r="205" spans="8:8" s="47" customFormat="1">
+      <c r="H205" s="45"/>
+    </row>
+    <row r="206" spans="8:8" s="47" customFormat="1">
+      <c r="H206" s="45"/>
+    </row>
+    <row r="207" spans="8:8" s="47" customFormat="1">
+      <c r="H207" s="45"/>
+    </row>
+    <row r="208" spans="8:8" s="47" customFormat="1">
+      <c r="H208" s="45"/>
+    </row>
+    <row r="209" spans="8:8" s="47" customFormat="1">
+      <c r="H209" s="45"/>
+    </row>
+    <row r="210" spans="8:8" s="47" customFormat="1">
+      <c r="H210" s="45"/>
+    </row>
+    <row r="211" spans="8:8" s="47" customFormat="1">
+      <c r="H211" s="45"/>
+    </row>
+    <row r="212" spans="8:8" s="47" customFormat="1">
+      <c r="H212" s="45"/>
+    </row>
+    <row r="213" spans="8:8" s="47" customFormat="1">
+      <c r="H213" s="45"/>
+    </row>
+    <row r="214" spans="8:8" s="47" customFormat="1">
+      <c r="H214" s="45"/>
+    </row>
+    <row r="215" spans="8:8" s="47" customFormat="1">
+      <c r="H215" s="45"/>
+    </row>
+    <row r="216" spans="8:8" s="47" customFormat="1">
+      <c r="H216" s="45"/>
+    </row>
+    <row r="217" spans="8:8" s="47" customFormat="1">
+      <c r="H217" s="45"/>
+    </row>
+    <row r="218" spans="8:8" s="47" customFormat="1">
+      <c r="H218" s="45"/>
+    </row>
+    <row r="219" spans="8:8" s="47" customFormat="1">
+      <c r="H219" s="45"/>
+    </row>
+    <row r="220" spans="8:8" s="47" customFormat="1">
+      <c r="H220" s="45"/>
+    </row>
+    <row r="221" spans="8:8" s="47" customFormat="1">
+      <c r="H221" s="45"/>
+    </row>
+    <row r="222" spans="8:8" s="47" customFormat="1">
+      <c r="H222" s="45"/>
+    </row>
+    <row r="223" spans="8:8" s="47" customFormat="1">
+      <c r="H223" s="45"/>
+    </row>
+    <row r="224" spans="8:8" s="47" customFormat="1">
+      <c r="H224" s="45"/>
+    </row>
+    <row r="225" spans="8:8" s="47" customFormat="1">
+      <c r="H225" s="45"/>
+    </row>
+    <row r="226" spans="8:8" s="47" customFormat="1">
+      <c r="H226" s="45"/>
+    </row>
+    <row r="227" spans="8:8" s="47" customFormat="1">
+      <c r="H227" s="45"/>
+    </row>
+    <row r="228" spans="8:8" s="47" customFormat="1">
+      <c r="H228" s="45"/>
+    </row>
+    <row r="229" spans="8:8" s="47" customFormat="1">
+      <c r="H229" s="45"/>
+    </row>
+    <row r="230" spans="8:8" s="47" customFormat="1">
+      <c r="H230" s="45"/>
+    </row>
+    <row r="231" spans="8:8" s="47" customFormat="1">
+      <c r="H231" s="45"/>
+    </row>
+    <row r="232" spans="8:8" s="47" customFormat="1">
+      <c r="H232" s="45"/>
+    </row>
+    <row r="233" spans="8:8" s="47" customFormat="1">
+      <c r="H233" s="45"/>
+    </row>
+    <row r="234" spans="8:8" s="47" customFormat="1">
+      <c r="H234" s="45"/>
+    </row>
+    <row r="235" spans="8:8" s="47" customFormat="1">
+      <c r="H235" s="45"/>
+    </row>
+    <row r="236" spans="8:8" s="47" customFormat="1">
+      <c r="H236" s="45"/>
+    </row>
+    <row r="237" spans="8:8" s="47" customFormat="1">
+      <c r="H237" s="45"/>
+    </row>
+    <row r="238" spans="8:8" s="47" customFormat="1">
+      <c r="H238" s="45"/>
+    </row>
+    <row r="239" spans="8:8" s="47" customFormat="1">
+      <c r="H239" s="45"/>
+    </row>
+    <row r="240" spans="8:8" s="47" customFormat="1">
+      <c r="H240" s="45"/>
+    </row>
+    <row r="241" spans="8:8" s="47" customFormat="1">
+      <c r="H241" s="45"/>
+    </row>
+    <row r="242" spans="8:8" s="47" customFormat="1">
+      <c r="H242" s="45"/>
+    </row>
+    <row r="243" spans="8:8" s="47" customFormat="1">
+      <c r="H243" s="45"/>
+    </row>
+    <row r="244" spans="8:8" s="47" customFormat="1">
+      <c r="H244" s="45"/>
+    </row>
+    <row r="245" spans="8:8" s="47" customFormat="1">
+      <c r="H245" s="45"/>
+    </row>
+    <row r="246" spans="8:8" s="47" customFormat="1">
+      <c r="H246" s="45"/>
+    </row>
+    <row r="247" spans="8:8" s="47" customFormat="1">
+      <c r="H247" s="45"/>
+    </row>
+    <row r="248" spans="8:8" s="47" customFormat="1">
+      <c r="H248" s="45"/>
+    </row>
+    <row r="249" spans="8:8" s="47" customFormat="1">
+      <c r="H249" s="45"/>
+    </row>
+    <row r="250" spans="8:8" s="47" customFormat="1">
+      <c r="H250" s="45"/>
+    </row>
+    <row r="251" spans="8:8" s="47" customFormat="1">
+      <c r="H251" s="45"/>
+    </row>
+    <row r="252" spans="8:8" s="47" customFormat="1">
+      <c r="H252" s="45"/>
+    </row>
+    <row r="253" spans="8:8" s="47" customFormat="1">
+      <c r="H253" s="45"/>
+    </row>
+    <row r="254" spans="8:8" s="47" customFormat="1">
+      <c r="H254" s="45"/>
+    </row>
+    <row r="255" spans="8:8" s="47" customFormat="1">
+      <c r="H255" s="45"/>
+    </row>
+    <row r="256" spans="8:8" s="47" customFormat="1">
+      <c r="H256" s="45"/>
+    </row>
+    <row r="257" spans="8:8" s="47" customFormat="1">
+      <c r="H257" s="45"/>
+    </row>
+    <row r="258" spans="8:8" s="47" customFormat="1">
+      <c r="H258" s="45"/>
+    </row>
+    <row r="259" spans="8:8" s="47" customFormat="1">
+      <c r="H259" s="45"/>
+    </row>
+    <row r="260" spans="8:8" s="47" customFormat="1">
+      <c r="H260" s="45"/>
+    </row>
+    <row r="261" spans="8:8" s="47" customFormat="1">
+      <c r="H261" s="45"/>
+    </row>
+    <row r="262" spans="8:8" s="47" customFormat="1">
+      <c r="H262" s="45"/>
+    </row>
+    <row r="263" spans="8:8" s="47" customFormat="1">
+      <c r="H263" s="45"/>
+    </row>
+    <row r="264" spans="8:8" s="47" customFormat="1">
+      <c r="H264" s="45"/>
+    </row>
+    <row r="265" spans="8:8" s="47" customFormat="1">
+      <c r="H265" s="45"/>
+    </row>
+    <row r="266" spans="8:8" s="47" customFormat="1">
+      <c r="H266" s="45"/>
+    </row>
+    <row r="267" spans="8:8" s="47" customFormat="1">
+      <c r="H267" s="45"/>
+    </row>
+    <row r="268" spans="8:8" s="47" customFormat="1">
+      <c r="H268" s="45"/>
+    </row>
+    <row r="269" spans="8:8" s="47" customFormat="1">
+      <c r="H269" s="45"/>
+    </row>
+    <row r="270" spans="8:8" s="47" customFormat="1">
+      <c r="H270" s="45"/>
+    </row>
+    <row r="271" spans="8:8" s="47" customFormat="1">
+      <c r="H271" s="45"/>
+    </row>
+    <row r="272" spans="8:8" s="47" customFormat="1">
+      <c r="H272" s="45"/>
+    </row>
+    <row r="273" spans="8:8" s="47" customFormat="1">
+      <c r="H273" s="45"/>
+    </row>
+    <row r="274" spans="8:8" s="47" customFormat="1">
+      <c r="H274" s="45"/>
+    </row>
+    <row r="275" spans="8:8" s="47" customFormat="1">
+      <c r="H275" s="45"/>
+    </row>
+    <row r="276" spans="8:8" s="47" customFormat="1">
+      <c r="H276" s="45"/>
+    </row>
+    <row r="277" spans="8:8" s="47" customFormat="1">
+      <c r="H277" s="45"/>
+    </row>
+    <row r="278" spans="8:8" s="47" customFormat="1">
+      <c r="H278" s="45"/>
+    </row>
+    <row r="279" spans="8:8" s="47" customFormat="1">
+      <c r="H279" s="45"/>
+    </row>
+    <row r="280" spans="8:8" s="47" customFormat="1">
+      <c r="H280" s="45"/>
+    </row>
+    <row r="281" spans="8:8" s="47" customFormat="1">
+      <c r="H281" s="45"/>
+    </row>
+    <row r="282" spans="8:8" s="47" customFormat="1">
+      <c r="H282" s="45"/>
+    </row>
+    <row r="283" spans="8:8" s="47" customFormat="1">
+      <c r="H283" s="45"/>
+    </row>
+    <row r="284" spans="8:8" s="47" customFormat="1">
+      <c r="H284" s="45"/>
+    </row>
+    <row r="285" spans="8:8" s="47" customFormat="1">
+      <c r="H285" s="45"/>
+    </row>
+    <row r="286" spans="8:8" s="47" customFormat="1">
+      <c r="H286" s="45"/>
+    </row>
+    <row r="287" spans="8:8" s="47" customFormat="1">
+      <c r="H287" s="45"/>
+    </row>
+    <row r="288" spans="8:8" s="47" customFormat="1">
+      <c r="H288" s="45"/>
+    </row>
+    <row r="289" spans="8:8" s="47" customFormat="1">
+      <c r="H289" s="45"/>
+    </row>
+    <row r="290" spans="8:8" s="47" customFormat="1">
+      <c r="H290" s="45"/>
+    </row>
+    <row r="291" spans="8:8" s="47" customFormat="1">
+      <c r="H291" s="45"/>
+    </row>
+    <row r="292" spans="8:8" s="47" customFormat="1">
+      <c r="H292" s="45"/>
+    </row>
+    <row r="293" spans="8:8" s="47" customFormat="1">
+      <c r="H293" s="45"/>
+    </row>
+    <row r="294" spans="8:8" s="47" customFormat="1">
+      <c r="H294" s="45"/>
+    </row>
+    <row r="295" spans="8:8" s="47" customFormat="1">
+      <c r="H295" s="45"/>
+    </row>
+    <row r="296" spans="8:8" s="47" customFormat="1">
+      <c r="H296" s="45"/>
+    </row>
+    <row r="297" spans="8:8" s="47" customFormat="1">
+      <c r="H297" s="45"/>
+    </row>
+    <row r="298" spans="8:8" s="47" customFormat="1">
+      <c r="H298" s="45"/>
+    </row>
+    <row r="299" spans="8:8" s="47" customFormat="1">
+      <c r="H299" s="45"/>
+    </row>
+    <row r="300" spans="8:8" s="47" customFormat="1">
+      <c r="H300" s="45"/>
+    </row>
+    <row r="301" spans="8:8" s="47" customFormat="1">
+      <c r="H301" s="45"/>
+    </row>
+    <row r="302" spans="8:8" s="47" customFormat="1">
+      <c r="H302" s="45"/>
+    </row>
+    <row r="303" spans="8:8" s="47" customFormat="1">
+      <c r="H303" s="45"/>
+    </row>
+    <row r="304" spans="8:8" s="47" customFormat="1">
+      <c r="H304" s="45"/>
+    </row>
+    <row r="305" spans="8:8" s="47" customFormat="1">
+      <c r="H305" s="45"/>
+    </row>
+    <row r="306" spans="8:8" s="47" customFormat="1">
+      <c r="H306" s="45"/>
+    </row>
+    <row r="307" spans="8:8" s="47" customFormat="1">
+      <c r="H307" s="45"/>
+    </row>
+    <row r="308" spans="8:8" s="47" customFormat="1">
+      <c r="H308" s="45"/>
+    </row>
+    <row r="309" spans="8:8" s="47" customFormat="1">
+      <c r="H309" s="45"/>
+    </row>
+    <row r="310" spans="8:8" s="47" customFormat="1">
+      <c r="H310" s="45"/>
+    </row>
+    <row r="311" spans="8:8" s="47" customFormat="1">
+      <c r="H311" s="45"/>
+    </row>
+    <row r="312" spans="8:8" s="47" customFormat="1">
+      <c r="H312" s="45"/>
+    </row>
+    <row r="313" spans="8:8" s="47" customFormat="1">
+      <c r="H313" s="45"/>
+    </row>
+    <row r="314" spans="8:8" s="47" customFormat="1">
+      <c r="H314" s="45"/>
+    </row>
+    <row r="315" spans="8:8" s="47" customFormat="1">
+      <c r="H315" s="45"/>
+    </row>
+    <row r="316" spans="8:8" s="47" customFormat="1">
+      <c r="H316" s="45"/>
+    </row>
+    <row r="317" spans="8:8" s="47" customFormat="1">
+      <c r="H317" s="45"/>
+    </row>
+    <row r="318" spans="8:8" s="47" customFormat="1">
+      <c r="H318" s="45"/>
+    </row>
+    <row r="319" spans="8:8" s="47" customFormat="1">
+      <c r="H319" s="45"/>
+    </row>
+    <row r="320" spans="8:8" s="47" customFormat="1">
+      <c r="H320" s="45"/>
+    </row>
+    <row r="321" spans="8:8" s="47" customFormat="1">
+      <c r="H321" s="45"/>
+    </row>
+    <row r="322" spans="8:8" s="47" customFormat="1">
+      <c r="H322" s="45"/>
+    </row>
+    <row r="323" spans="8:8" s="47" customFormat="1">
+      <c r="H323" s="45"/>
+    </row>
+    <row r="324" spans="8:8" s="47" customFormat="1">
+      <c r="H324" s="45"/>
+    </row>
+    <row r="325" spans="8:8" s="47" customFormat="1">
+      <c r="H325" s="45"/>
+    </row>
+    <row r="326" spans="8:8" s="47" customFormat="1">
+      <c r="H326" s="45"/>
+    </row>
+    <row r="327" spans="8:8" s="47" customFormat="1">
+      <c r="H327" s="45"/>
+    </row>
+    <row r="328" spans="8:8" s="47" customFormat="1">
+      <c r="H328" s="45"/>
+    </row>
+    <row r="329" spans="8:8" s="47" customFormat="1">
+      <c r="H329" s="45"/>
+    </row>
+    <row r="330" spans="8:8" s="47" customFormat="1">
+      <c r="H330" s="45"/>
+    </row>
+    <row r="331" spans="8:8" s="47" customFormat="1">
+      <c r="H331" s="45"/>
+    </row>
+    <row r="332" spans="8:8" s="47" customFormat="1">
+      <c r="H332" s="45"/>
+    </row>
+    <row r="333" spans="8:8" s="47" customFormat="1">
+      <c r="H333" s="45"/>
+    </row>
+    <row r="334" spans="8:8" s="47" customFormat="1">
+      <c r="H334" s="45"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2855,19 +3458,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" style="17" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="17" width="10.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="17" width="12.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="17" width="14.7109375" collapsed="true"/>
-    <col min="5" max="6" customWidth="true" style="17" width="10.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="17" width="21.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="17" width="12.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="17" width="24.85546875" collapsed="true"/>
-    <col min="10" max="10" style="17" width="9.140625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="17" width="14.7109375" collapsed="true"/>
-    <col min="12" max="13" customWidth="true" style="17" width="14.0" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="17" width="22.42578125" collapsed="true"/>
-    <col min="15" max="16384" style="17" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="17" collapsed="1"/>
+    <col min="2" max="2" width="10.7109375" style="17" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.28515625" style="17" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.7109375" style="17" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="10" style="17" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21" style="17" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.5703125" style="17" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="24.85546875" style="17" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="9.140625" style="17" collapsed="1"/>
+    <col min="11" max="11" width="14.7109375" style="17" customWidth="1" collapsed="1"/>
+    <col min="12" max="13" width="14" style="17" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="22.42578125" style="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="16384" width="9.140625" style="17" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="3" customFormat="1" ht="21.75" customHeight="1">
@@ -3174,15 +3777,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="37" width="27.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="37" width="9.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="37" width="14.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="37" width="12.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="37" width="38.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="39" width="13.28515625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="39" width="13.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="37" width="11.7109375" collapsed="true"/>
-    <col min="9" max="16384" style="37" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="27.140625" style="37" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.5703125" style="37" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14" style="37" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.140625" style="37" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="38.5703125" style="37" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.28515625" style="39" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.42578125" style="39" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.7109375" style="37" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="9.140625" style="37" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="39" customFormat="1" ht="22.5" customHeight="1">
@@ -3849,8 +4452,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="7.85546875" collapsed="true"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="7.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="12.75" customHeight="1">
@@ -3887,7 +4490,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="2" max="6" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="2" max="6" width="24.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -4153,8 +4756,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="7" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="1" max="7" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75">

</xml_diff>

<commit_message>
commiting with duplicacy issue in report in case of multiple modules
</commit_message>
<xml_diff>
--- a/src/TestData/Add_Appointment_Suite.xlsx
+++ b/src/TestData/Add_Appointment_Suite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14295" windowHeight="6135" tabRatio="700" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14295" windowHeight="6135" tabRatio="700" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="12" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="261">
   <si>
     <t>Browser</t>
   </si>
@@ -798,6 +798,15 @@
   </si>
   <si>
     <t>Navigate to google.com</t>
+  </si>
+  <si>
+    <t>Navigate to fb.com</t>
+  </si>
+  <si>
+    <t>checking appointment</t>
+  </si>
+  <si>
+    <t>Click on fb login button</t>
   </si>
 </sst>
 </file>
@@ -1932,8 +1941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2028,7 +2037,7 @@
         <v>230</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>74</v>
+        <v>259</v>
       </c>
       <c r="E4" s="18" t="s">
         <v>8</v>
@@ -2051,7 +2060,7 @@
         <v>231</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>74</v>
+        <v>231</v>
       </c>
       <c r="E5" s="18" t="s">
         <v>8</v>
@@ -2074,7 +2083,7 @@
         <v>235</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>74</v>
+        <v>258</v>
       </c>
       <c r="E6" s="18" t="s">
         <v>13</v>
@@ -2096,8 +2105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V334"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2421,8 +2430,8 @@
       <c r="N9" s="61"/>
     </row>
     <row r="10" spans="1:22" s="46" customFormat="1">
-      <c r="A10" s="46" t="s">
-        <v>93</v>
+      <c r="A10" s="60" t="s">
+        <v>7</v>
       </c>
       <c r="C10" s="45">
         <v>9</v>
@@ -2441,12 +2450,15 @@
       <c r="S10" s="53"/>
     </row>
     <row r="11" spans="1:22" s="46" customFormat="1">
-      <c r="A11" s="46" t="s">
+      <c r="A11" s="60" t="s">
         <v>93</v>
       </c>
       <c r="C11" s="45">
         <v>10</v>
       </c>
+      <c r="D11" s="46" t="s">
+        <v>260</v>
+      </c>
       <c r="E11" s="46" t="s">
         <v>168</v>
       </c>
@@ -2455,7 +2467,7 @@
       </c>
       <c r="H11" s="45"/>
       <c r="K11" s="46" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="R11" s="53"/>
       <c r="S11" s="53"/>

</xml_diff>

<commit_message>
report duplicacy of previous module data resolved
</commit_message>
<xml_diff>
--- a/src/TestData/Add_Appointment_Suite.xlsx
+++ b/src/TestData/Add_Appointment_Suite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14295" windowHeight="6135" tabRatio="700" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14295" windowHeight="6135" tabRatio="700" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="12" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="261">
   <si>
     <t>Browser</t>
   </si>
@@ -1941,7 +1941,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -2105,8 +2105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V334"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2366,7 +2366,7 @@
         <v>246</v>
       </c>
       <c r="K7" s="45" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="L7" s="51"/>
       <c r="M7" s="51"/>
@@ -2473,6 +2473,12 @@
       <c r="S11" s="53"/>
     </row>
     <row r="12" spans="1:22" s="47" customFormat="1">
+      <c r="A12" s="60" t="s">
+        <v>93</v>
+      </c>
+      <c r="E12" s="38" t="s">
+        <v>221</v>
+      </c>
       <c r="H12" s="45"/>
       <c r="I12" s="48"/>
       <c r="J12" s="48"/>
@@ -3783,8 +3789,8 @@
   <dimension ref="A1:J66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>

</xml_diff>

<commit_message>
Commiting code with changes made for starting implementation for Prerequisites and applicationSpecific class related changes as discussed with vikas on tuesday
</commit_message>
<xml_diff>
--- a/src/TestData/Add_Appointment_Suite.xlsx
+++ b/src/TestData/Add_Appointment_Suite.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="258">
   <si>
     <t>Browser</t>
   </si>
@@ -722,21 +722,12 @@
     <t>register patient</t>
   </si>
   <si>
-    <t>testsiteBaseURL2</t>
-  </si>
-  <si>
-    <t>testsiteBaseURL3</t>
-  </si>
-  <si>
     <t>navigate to google</t>
   </si>
   <si>
     <t>navigate to fb</t>
   </si>
   <si>
-    <t>button_login_fb</t>
-  </si>
-  <si>
     <t>Method Name</t>
   </si>
   <si>
@@ -758,21 +749,12 @@
     <t>Click on login button</t>
   </si>
   <si>
-    <t>verify login</t>
-  </si>
-  <si>
     <t>waitForPageLoad</t>
   </si>
   <si>
     <t>page_load_wait_time</t>
   </si>
   <si>
-    <t>todays_appointment_text</t>
-  </si>
-  <si>
-    <t>todays_appointment_text_path</t>
-  </si>
-  <si>
     <t>Suite</t>
   </si>
   <si>
@@ -794,9 +776,6 @@
     <t>Logging into PRM</t>
   </si>
   <si>
-    <t>Navigate to test url</t>
-  </si>
-  <si>
     <t>Navigate to google.com</t>
   </si>
   <si>
@@ -806,7 +785,19 @@
     <t>checking appointment</t>
   </si>
   <si>
-    <t>Click on fb login button</t>
+    <t>Wait for the page to load</t>
+  </si>
+  <si>
+    <t>patientID</t>
+  </si>
+  <si>
+    <t>gsearch</t>
+  </si>
+  <si>
+    <t>gbtn</t>
+  </si>
+  <si>
+    <t>Class</t>
   </si>
 </sst>
 </file>
@@ -1942,7 +1933,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1959,7 +1950,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="22.5" customHeight="1">
       <c r="A1" s="19" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>177</v>
@@ -1974,7 +1965,7 @@
         <v>11</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>9</v>
+        <v>257</v>
       </c>
       <c r="G1" s="19" t="s">
         <v>29</v>
@@ -1982,7 +1973,7 @@
     </row>
     <row r="2" spans="1:7" ht="22.5" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>2</v>
@@ -1991,13 +1982,13 @@
         <v>229</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>74</v>
+        <v>6</v>
       </c>
       <c r="G2" s="18" t="s">
         <v>13</v>
@@ -2005,19 +1996,19 @@
     </row>
     <row r="3" spans="1:7" ht="22.5" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="B3" s="18" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F3" s="18" t="s">
         <v>74</v>
@@ -2028,7 +2019,7 @@
     </row>
     <row r="4" spans="1:7" ht="22.5" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>12</v>
@@ -2037,7 +2028,7 @@
         <v>230</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="E4" s="18" t="s">
         <v>8</v>
@@ -2051,7 +2042,7 @@
     </row>
     <row r="5" spans="1:7" ht="22.5" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>16</v>
@@ -2074,19 +2065,19 @@
     </row>
     <row r="6" spans="1:7" ht="22.5" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
@@ -2103,10 +2094,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V334"/>
+  <dimension ref="A1:V335"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2115,7 +2106,7 @@
     <col min="2" max="2" width="9.5703125" style="44" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="6.7109375" style="44" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="29" style="44" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.42578125" style="44" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="26.85546875" style="44" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="25.7109375" style="44" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="31.28515625" style="44" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="11.7109375" style="45" customWidth="1" collapsed="1"/>
@@ -2223,7 +2214,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="45" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E3" s="45" t="s">
         <v>167</v>
@@ -2260,7 +2251,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="45" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E4" s="45" t="s">
         <v>169</v>
@@ -2332,7 +2323,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="45" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E6" s="45" t="s">
         <v>168</v>
@@ -2360,13 +2351,13 @@
         <v>6</v>
       </c>
       <c r="E7" s="45" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="F7" s="45" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="K7" s="45" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="L7" s="51"/>
       <c r="M7" s="51"/>
@@ -2384,17 +2375,14 @@
       <c r="C8" s="45">
         <v>7</v>
       </c>
-      <c r="D8" s="45" t="s">
-        <v>244</v>
-      </c>
       <c r="E8" s="45" t="s">
-        <v>206</v>
+        <v>169</v>
       </c>
       <c r="F8" s="45" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="G8" s="45" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="K8" s="45" t="s">
         <v>13</v>
@@ -2408,148 +2396,116 @@
       <c r="U8" s="51"/>
       <c r="V8" s="51"/>
     </row>
-    <row r="9" spans="1:22" s="60" customFormat="1">
-      <c r="A9" s="60" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="60">
-        <v>8</v>
-      </c>
-      <c r="D9" s="60" t="s">
+    <row r="9" spans="1:22" s="45" customFormat="1" ht="18" customHeight="1">
+      <c r="A9" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="45" t="s">
+        <v>168</v>
+      </c>
+      <c r="G9" s="45" t="s">
         <v>256</v>
       </c>
-      <c r="E9" s="60" t="s">
-        <v>167</v>
-      </c>
-      <c r="F9" s="60" t="s">
-        <v>232</v>
-      </c>
-      <c r="K9" s="60" t="s">
+      <c r="K9" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="N9" s="61"/>
-    </row>
-    <row r="10" spans="1:22" s="46" customFormat="1">
-      <c r="A10" s="60" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="45">
-        <v>9</v>
-      </c>
-      <c r="E10" s="46" t="s">
-        <v>167</v>
-      </c>
-      <c r="F10" s="46" t="s">
-        <v>233</v>
-      </c>
-      <c r="H10" s="45"/>
-      <c r="K10" s="46" t="s">
-        <v>13</v>
-      </c>
-      <c r="R10" s="53"/>
-      <c r="S10" s="53"/>
+      <c r="L9" s="51"/>
+      <c r="M9" s="51"/>
+      <c r="N9" s="51"/>
+      <c r="R9" s="51"/>
+      <c r="S9" s="51"/>
+      <c r="T9" s="51"/>
+      <c r="U9" s="51"/>
+      <c r="V9" s="51"/>
+    </row>
+    <row r="10" spans="1:22" s="60" customFormat="1">
+      <c r="N10" s="61"/>
     </row>
     <row r="11" spans="1:22" s="46" customFormat="1">
-      <c r="A11" s="60" t="s">
-        <v>93</v>
-      </c>
-      <c r="C11" s="45">
-        <v>10</v>
-      </c>
-      <c r="D11" s="46" t="s">
-        <v>260</v>
-      </c>
-      <c r="E11" s="46" t="s">
-        <v>168</v>
-      </c>
-      <c r="G11" s="46" t="s">
-        <v>236</v>
-      </c>
+      <c r="A11" s="60"/>
+      <c r="C11" s="45"/>
       <c r="H11" s="45"/>
-      <c r="K11" s="46" t="s">
-        <v>13</v>
-      </c>
       <c r="R11" s="53"/>
       <c r="S11" s="53"/>
     </row>
-    <row r="12" spans="1:22" s="47" customFormat="1">
-      <c r="A12" s="60" t="s">
-        <v>93</v>
-      </c>
-      <c r="E12" s="38" t="s">
-        <v>221</v>
-      </c>
+    <row r="12" spans="1:22" s="46" customFormat="1">
+      <c r="A12" s="60"/>
+      <c r="C12" s="45"/>
       <c r="H12" s="45"/>
-      <c r="I12" s="48"/>
-      <c r="J12" s="48"/>
-      <c r="K12" s="48"/>
-      <c r="L12" s="48"/>
-      <c r="M12" s="48"/>
+      <c r="R12" s="53"/>
+      <c r="S12" s="53"/>
     </row>
     <row r="13" spans="1:22" s="47" customFormat="1">
+      <c r="A13" s="60"/>
+      <c r="E13" s="38"/>
       <c r="H13" s="45"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="48"/>
+      <c r="K13" s="48"/>
+      <c r="L13" s="48"/>
+      <c r="M13" s="48"/>
     </row>
     <row r="14" spans="1:22" s="47" customFormat="1">
       <c r="H14" s="45"/>
     </row>
     <row r="15" spans="1:22" s="47" customFormat="1">
-      <c r="E15" s="52"/>
       <c r="H15" s="45"/>
     </row>
     <row r="16" spans="1:22" s="47" customFormat="1">
       <c r="E16" s="52"/>
       <c r="H16" s="45"/>
     </row>
-    <row r="17" spans="6:8" s="47" customFormat="1">
+    <row r="17" spans="5:8" s="47" customFormat="1">
+      <c r="E17" s="52"/>
       <c r="H17" s="45"/>
     </row>
-    <row r="18" spans="6:8" s="47" customFormat="1">
+    <row r="18" spans="5:8" s="47" customFormat="1">
       <c r="H18" s="45"/>
     </row>
-    <row r="19" spans="6:8" s="47" customFormat="1">
+    <row r="19" spans="5:8" s="47" customFormat="1">
       <c r="H19" s="45"/>
     </row>
-    <row r="20" spans="6:8" s="47" customFormat="1">
+    <row r="20" spans="5:8" s="47" customFormat="1">
       <c r="H20" s="45"/>
     </row>
-    <row r="21" spans="6:8" s="47" customFormat="1">
+    <row r="21" spans="5:8" s="47" customFormat="1">
       <c r="H21" s="45"/>
     </row>
-    <row r="22" spans="6:8" s="47" customFormat="1">
+    <row r="22" spans="5:8" s="47" customFormat="1">
       <c r="H22" s="45"/>
     </row>
-    <row r="23" spans="6:8" s="47" customFormat="1">
+    <row r="23" spans="5:8" s="47" customFormat="1">
       <c r="H23" s="45"/>
     </row>
-    <row r="24" spans="6:8" s="47" customFormat="1">
+    <row r="24" spans="5:8" s="47" customFormat="1">
       <c r="H24" s="45"/>
     </row>
-    <row r="25" spans="6:8" s="47" customFormat="1">
-      <c r="F25" s="49"/>
-      <c r="G25" s="50"/>
+    <row r="25" spans="5:8" s="47" customFormat="1">
       <c r="H25" s="45"/>
     </row>
-    <row r="26" spans="6:8" s="47" customFormat="1">
+    <row r="26" spans="5:8" s="47" customFormat="1">
+      <c r="F26" s="49"/>
+      <c r="G26" s="50"/>
       <c r="H26" s="45"/>
     </row>
-    <row r="27" spans="6:8" s="47" customFormat="1">
+    <row r="27" spans="5:8" s="47" customFormat="1">
       <c r="H27" s="45"/>
     </row>
-    <row r="28" spans="6:8" s="47" customFormat="1">
+    <row r="28" spans="5:8" s="47" customFormat="1">
       <c r="H28" s="45"/>
     </row>
-    <row r="29" spans="6:8" s="47" customFormat="1">
+    <row r="29" spans="5:8" s="47" customFormat="1">
       <c r="H29" s="45"/>
     </row>
-    <row r="30" spans="6:8" s="47" customFormat="1">
+    <row r="30" spans="5:8" s="47" customFormat="1">
       <c r="H30" s="45"/>
     </row>
-    <row r="31" spans="6:8" s="47" customFormat="1">
-      <c r="F31" s="49"/>
-      <c r="G31" s="50"/>
+    <row r="31" spans="5:8" s="47" customFormat="1">
       <c r="H31" s="45"/>
     </row>
-    <row r="32" spans="6:8" s="47" customFormat="1">
+    <row r="32" spans="5:8" s="47" customFormat="1">
+      <c r="F32" s="49"/>
+      <c r="G32" s="50"/>
       <c r="H32" s="45"/>
     </row>
     <row r="33" spans="8:8" s="47" customFormat="1">
@@ -3457,6 +3413,9 @@
     </row>
     <row r="334" spans="8:8" s="47" customFormat="1">
       <c r="H334" s="45"/>
+    </row>
+    <row r="335" spans="8:8" s="47" customFormat="1">
+      <c r="H335" s="45"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -3789,8 +3748,8 @@
   <dimension ref="A1:J66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4298,11 +4257,21 @@
       </c>
     </row>
     <row r="29" spans="1:7" s="38" customFormat="1">
+      <c r="A29" s="38" t="s">
+        <v>241</v>
+      </c>
       <c r="C29" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="F29" s="42"/>
-      <c r="G29" s="42"/>
+      <c r="E29" s="38" t="s">
+        <v>253</v>
+      </c>
+      <c r="F29" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" s="42" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="30" spans="1:7" s="36" customFormat="1">
       <c r="F30" s="41"/>
@@ -4476,16 +4445,16 @@
   <sheetData>
     <row r="1" spans="1:5" ht="12.75" customHeight="1">
       <c r="A1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D1" t="s">
         <v>237</v>
-      </c>
-      <c r="B1" t="s">
-        <v>238</v>
-      </c>
-      <c r="C1" t="s">
-        <v>239</v>
-      </c>
-      <c r="D1" t="s">
-        <v>240</v>
       </c>
       <c r="E1" t="s">
         <v>165</v>

</xml_diff>

<commit_message>
divided driverscript into 2. Created excute keyword preq and appSpecific fn.
</commit_message>
<xml_diff>
--- a/src/TestData/Add_Appointment_Suite.xlsx
+++ b/src/TestData/Add_Appointment_Suite.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="261">
   <si>
     <t>Browser</t>
   </si>
@@ -92,18 +92,6 @@
     <t>Path</t>
   </si>
   <si>
-    <t>TD002</t>
-  </si>
-  <si>
-    <t>TD003</t>
-  </si>
-  <si>
-    <t>TD004</t>
-  </si>
-  <si>
-    <t>TD005</t>
-  </si>
-  <si>
     <t>Test Step Desc</t>
   </si>
   <si>
@@ -281,9 +269,6 @@
     <t>Los Angeles</t>
   </si>
   <si>
-    <t>New York</t>
-  </si>
-  <si>
     <t>qtp</t>
   </si>
   <si>
@@ -308,9 +293,6 @@
     <t>TC005</t>
   </si>
   <si>
-    <t>iexplore.exe</t>
-  </si>
-  <si>
     <t>Reusable keyword funtions using DP</t>
   </si>
   <si>
@@ -443,9 +425,6 @@
     <t>SearchText</t>
   </si>
   <si>
-    <t>Search Results</t>
-  </si>
-  <si>
     <t>Zipcode</t>
   </si>
   <si>
@@ -476,33 +455,18 @@
     <t>player123@yopmail.com</t>
   </si>
   <si>
-    <t>Gc1234564</t>
-  </si>
-  <si>
     <t>LastName</t>
   </si>
   <si>
     <t>FirstName</t>
   </si>
   <si>
-    <t>Sinha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Result </t>
-  </si>
-  <si>
     <t>Country</t>
   </si>
   <si>
     <t>USA</t>
   </si>
   <si>
-    <t>Noida</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
     <t>Height</t>
   </si>
   <si>
@@ -788,16 +752,61 @@
     <t>Wait for the page to load</t>
   </si>
   <si>
-    <t>patientID</t>
-  </si>
-  <si>
-    <t>gsearch</t>
-  </si>
-  <si>
-    <t>gbtn</t>
-  </si>
-  <si>
     <t>Class</t>
+  </si>
+  <si>
+    <t>TC006</t>
+  </si>
+  <si>
+    <t>TC007</t>
+  </si>
+  <si>
+    <t>TC008</t>
+  </si>
+  <si>
+    <t>TC009</t>
+  </si>
+  <si>
+    <t>TC010</t>
+  </si>
+  <si>
+    <t>TC011</t>
+  </si>
+  <si>
+    <t>TC012</t>
+  </si>
+  <si>
+    <t>TC013</t>
+  </si>
+  <si>
+    <t>TC014</t>
+  </si>
+  <si>
+    <t>TC015</t>
+  </si>
+  <si>
+    <t>Mozilla</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Cena</t>
+  </si>
+  <si>
+    <t>clovedental@clove.in</t>
+  </si>
+  <si>
+    <t>Doctor</t>
+  </si>
+  <si>
+    <t>Amit Dua</t>
+  </si>
+  <si>
+    <t>addAppointment</t>
+  </si>
+  <si>
+    <t>www.google.com</t>
   </si>
 </sst>
 </file>
@@ -1508,81 +1517,81 @@
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="B11" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="6" customFormat="1" ht="42" customHeight="1">
       <c r="A12" s="5" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="18" customHeight="1">
@@ -1590,7 +1599,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C13" s="31">
         <v>0.75</v>
@@ -1602,7 +1611,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C14" s="31">
         <v>0.5</v>
@@ -1613,7 +1622,7 @@
         <v>3</v>
       </c>
       <c r="B15" s="32" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C15" s="31">
         <v>0.5</v>
@@ -1624,7 +1633,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C16" s="7">
         <v>0.5</v>
@@ -1635,7 +1644,7 @@
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C17" s="7">
         <v>0.75</v>
@@ -1646,7 +1655,7 @@
         <v>6</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C18" s="7">
         <v>0.75</v>
@@ -1657,7 +1666,7 @@
         <v>7</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C19" s="7">
         <v>0.5</v>
@@ -1668,7 +1677,7 @@
         <v>8</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C20" s="7"/>
     </row>
@@ -1677,7 +1686,7 @@
         <v>9</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C21" s="7"/>
     </row>
@@ -1704,130 +1713,130 @@
     <row r="26" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="27" spans="1:3" ht="15.75" customHeight="1">
       <c r="A27" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" customHeight="1">
       <c r="A28" s="8"/>
       <c r="B28" s="9" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15.75" customHeight="1">
       <c r="A29" s="8"/>
       <c r="B29" s="9" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" customHeight="1">
       <c r="A30" s="8"/>
       <c r="B30" s="9" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" customHeight="1">
       <c r="A31" s="8"/>
       <c r="B31" s="9" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" customHeight="1">
       <c r="A32" s="8"/>
       <c r="B32" s="9" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" customHeight="1">
       <c r="A33" s="8"/>
       <c r="B33" s="9" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" customHeight="1">
       <c r="A34" s="8"/>
       <c r="B34" s="9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="15.75" customHeight="1">
       <c r="A35" s="8"/>
       <c r="B35" s="9" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15.75" customHeight="1">
       <c r="A36" s="8"/>
       <c r="B36" s="9" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15.75" customHeight="1">
       <c r="A37" s="8"/>
       <c r="B37" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="15.75" customHeight="1">
       <c r="A38" s="8"/>
       <c r="B38" s="9" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="15.75" customHeight="1">
       <c r="A39" s="8"/>
       <c r="B39" s="9" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15.75" customHeight="1">
       <c r="A40" s="8"/>
       <c r="B40" s="9" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="15.75" customHeight="1">
@@ -1840,40 +1849,40 @@
     </row>
     <row r="43" spans="1:3" ht="15.75" customHeight="1">
       <c r="A43" s="12" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B43" s="2"/>
     </row>
     <row r="44" spans="1:3" ht="15.75" customHeight="1">
       <c r="A44" s="13" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="15.75" customHeight="1">
       <c r="A45" s="2"/>
       <c r="B45" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="15.75" customHeight="1">
       <c r="A46" s="2"/>
       <c r="B46" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="15.75" customHeight="1">
       <c r="A47" s="2"/>
       <c r="B47" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1">
       <c r="A48" s="2"/>
       <c r="B48" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="15.75" customHeight="1">
@@ -1882,16 +1891,16 @@
     </row>
     <row r="50" spans="1:2" ht="15.75" customHeight="1">
       <c r="A50" s="13" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="15.75" customHeight="1">
       <c r="A51" s="2"/>
       <c r="B51" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15.75" customHeight="1"/>
@@ -1950,10 +1959,10 @@
   <sheetData>
     <row r="1" spans="1:7" ht="22.5" customHeight="1">
       <c r="A1" s="19" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="C1" s="19" t="s">
         <v>4</v>
@@ -1965,24 +1974,24 @@
         <v>11</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="22.5" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>13</v>
@@ -1996,22 +2005,22 @@
     </row>
     <row r="3" spans="1:7" ht="22.5" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="B3" s="18" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="E3" s="18" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G3" s="18" t="s">
         <v>13</v>
@@ -2019,22 +2028,22 @@
     </row>
     <row r="4" spans="1:7" ht="22.5" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="E4" s="18" t="s">
         <v>8</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G4" s="18" t="s">
         <v>13</v>
@@ -2042,22 +2051,22 @@
     </row>
     <row r="5" spans="1:7" ht="22.5" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="E5" s="18" t="s">
         <v>8</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G5" s="18" t="s">
         <v>13</v>
@@ -2065,16 +2074,16 @@
     </row>
     <row r="6" spans="1:7" ht="22.5" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="E6" s="18" t="s">
         <v>8</v>
@@ -2094,10 +2103,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V335"/>
+  <dimension ref="A1:V334"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7:K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2128,22 +2137,22 @@
         <v>3</v>
       </c>
       <c r="B1" s="54" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C1" s="54" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D1" s="54" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E1" s="54" t="s">
         <v>6</v>
       </c>
       <c r="F1" s="54" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="G1" s="54" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="H1" s="45" t="s">
         <v>9</v>
@@ -2152,7 +2161,7 @@
         <v>17</v>
       </c>
       <c r="J1" s="55" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="K1" s="55" t="s">
         <v>11</v>
@@ -2177,19 +2186,19 @@
         <v>1</v>
       </c>
       <c r="D2" s="45" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="E2" s="45" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="F2" s="45" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="I2" s="45" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="J2" s="45" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="K2" s="45" t="s">
         <v>13</v>
@@ -2214,19 +2223,19 @@
         <v>2</v>
       </c>
       <c r="D3" s="45" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="E3" s="45" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="F3" s="45" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="I3" s="45" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="J3" s="45" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="K3" s="45" t="s">
         <v>13</v>
@@ -2251,19 +2260,19 @@
         <v>3</v>
       </c>
       <c r="D4" s="45" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="E4" s="45" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="F4" s="45" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="G4" s="45" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="I4" s="45" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="K4" s="45" t="s">
         <v>13</v>
@@ -2288,19 +2297,19 @@
         <v>4</v>
       </c>
       <c r="D5" s="45" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="E5" s="45" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="F5" s="45" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="G5" s="45" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="I5" s="45" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="K5" s="45" t="s">
         <v>13</v>
@@ -2323,13 +2332,13 @@
         <v>5</v>
       </c>
       <c r="D6" s="45" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="E6" s="45" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="G6" s="45" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="K6" s="45" t="s">
         <v>13</v>
@@ -2351,10 +2360,10 @@
         <v>6</v>
       </c>
       <c r="E7" s="45" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="F7" s="45" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="K7" s="45" t="s">
         <v>13</v>
@@ -2376,18 +2385,11 @@
         <v>7</v>
       </c>
       <c r="E8" s="45" t="s">
-        <v>169</v>
-      </c>
-      <c r="F8" s="45" t="s">
-        <v>254</v>
-      </c>
-      <c r="G8" s="45" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="K8" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="L8" s="51"/>
       <c r="M8" s="51"/>
       <c r="N8" s="51"/>
       <c r="R8" s="51"/>
@@ -2396,30 +2398,15 @@
       <c r="U8" s="51"/>
       <c r="V8" s="51"/>
     </row>
-    <row r="9" spans="1:22" s="45" customFormat="1" ht="18" customHeight="1">
-      <c r="A9" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="45" t="s">
-        <v>168</v>
-      </c>
-      <c r="G9" s="45" t="s">
-        <v>256</v>
-      </c>
-      <c r="K9" s="45" t="s">
-        <v>13</v>
-      </c>
-      <c r="L9" s="51"/>
-      <c r="M9" s="51"/>
-      <c r="N9" s="51"/>
-      <c r="R9" s="51"/>
-      <c r="S9" s="51"/>
-      <c r="T9" s="51"/>
-      <c r="U9" s="51"/>
-      <c r="V9" s="51"/>
-    </row>
-    <row r="10" spans="1:22" s="60" customFormat="1">
-      <c r="N10" s="61"/>
+    <row r="9" spans="1:22" s="60" customFormat="1">
+      <c r="N9" s="61"/>
+    </row>
+    <row r="10" spans="1:22" s="46" customFormat="1">
+      <c r="A10" s="60"/>
+      <c r="C10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="R10" s="53"/>
+      <c r="S10" s="53"/>
     </row>
     <row r="11" spans="1:22" s="46" customFormat="1">
       <c r="A11" s="60"/>
@@ -2428,84 +2415,80 @@
       <c r="R11" s="53"/>
       <c r="S11" s="53"/>
     </row>
-    <row r="12" spans="1:22" s="46" customFormat="1">
+    <row r="12" spans="1:22" s="47" customFormat="1">
       <c r="A12" s="60"/>
-      <c r="C12" s="45"/>
+      <c r="E12" s="38"/>
       <c r="H12" s="45"/>
-      <c r="R12" s="53"/>
-      <c r="S12" s="53"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="48"/>
+      <c r="K12" s="48"/>
+      <c r="L12" s="48"/>
+      <c r="M12" s="48"/>
     </row>
     <row r="13" spans="1:22" s="47" customFormat="1">
-      <c r="A13" s="60"/>
-      <c r="E13" s="38"/>
       <c r="H13" s="45"/>
-      <c r="I13" s="48"/>
-      <c r="J13" s="48"/>
-      <c r="K13" s="48"/>
-      <c r="L13" s="48"/>
-      <c r="M13" s="48"/>
     </row>
     <row r="14" spans="1:22" s="47" customFormat="1">
       <c r="H14" s="45"/>
     </row>
     <row r="15" spans="1:22" s="47" customFormat="1">
+      <c r="E15" s="52"/>
       <c r="H15" s="45"/>
     </row>
     <row r="16" spans="1:22" s="47" customFormat="1">
       <c r="E16" s="52"/>
       <c r="H16" s="45"/>
     </row>
-    <row r="17" spans="5:8" s="47" customFormat="1">
-      <c r="E17" s="52"/>
+    <row r="17" spans="6:8" s="47" customFormat="1">
       <c r="H17" s="45"/>
     </row>
-    <row r="18" spans="5:8" s="47" customFormat="1">
+    <row r="18" spans="6:8" s="47" customFormat="1">
       <c r="H18" s="45"/>
     </row>
-    <row r="19" spans="5:8" s="47" customFormat="1">
+    <row r="19" spans="6:8" s="47" customFormat="1">
       <c r="H19" s="45"/>
     </row>
-    <row r="20" spans="5:8" s="47" customFormat="1">
+    <row r="20" spans="6:8" s="47" customFormat="1">
       <c r="H20" s="45"/>
     </row>
-    <row r="21" spans="5:8" s="47" customFormat="1">
+    <row r="21" spans="6:8" s="47" customFormat="1">
       <c r="H21" s="45"/>
     </row>
-    <row r="22" spans="5:8" s="47" customFormat="1">
+    <row r="22" spans="6:8" s="47" customFormat="1">
       <c r="H22" s="45"/>
     </row>
-    <row r="23" spans="5:8" s="47" customFormat="1">
+    <row r="23" spans="6:8" s="47" customFormat="1">
       <c r="H23" s="45"/>
     </row>
-    <row r="24" spans="5:8" s="47" customFormat="1">
+    <row r="24" spans="6:8" s="47" customFormat="1">
       <c r="H24" s="45"/>
     </row>
-    <row r="25" spans="5:8" s="47" customFormat="1">
+    <row r="25" spans="6:8" s="47" customFormat="1">
+      <c r="F25" s="49"/>
+      <c r="G25" s="50"/>
       <c r="H25" s="45"/>
     </row>
-    <row r="26" spans="5:8" s="47" customFormat="1">
-      <c r="F26" s="49"/>
-      <c r="G26" s="50"/>
+    <row r="26" spans="6:8" s="47" customFormat="1">
       <c r="H26" s="45"/>
     </row>
-    <row r="27" spans="5:8" s="47" customFormat="1">
+    <row r="27" spans="6:8" s="47" customFormat="1">
       <c r="H27" s="45"/>
     </row>
-    <row r="28" spans="5:8" s="47" customFormat="1">
+    <row r="28" spans="6:8" s="47" customFormat="1">
       <c r="H28" s="45"/>
     </row>
-    <row r="29" spans="5:8" s="47" customFormat="1">
+    <row r="29" spans="6:8" s="47" customFormat="1">
       <c r="H29" s="45"/>
     </row>
-    <row r="30" spans="5:8" s="47" customFormat="1">
+    <row r="30" spans="6:8" s="47" customFormat="1">
       <c r="H30" s="45"/>
     </row>
-    <row r="31" spans="5:8" s="47" customFormat="1">
+    <row r="31" spans="6:8" s="47" customFormat="1">
+      <c r="F31" s="49"/>
+      <c r="G31" s="50"/>
       <c r="H31" s="45"/>
     </row>
-    <row r="32" spans="5:8" s="47" customFormat="1">
-      <c r="F32" s="49"/>
-      <c r="G32" s="50"/>
+    <row r="32" spans="6:8" s="47" customFormat="1">
       <c r="H32" s="45"/>
     </row>
     <row r="33" spans="8:8" s="47" customFormat="1">
@@ -3413,9 +3396,6 @@
     </row>
     <row r="334" spans="8:8" s="47" customFormat="1">
       <c r="H334" s="45"/>
-    </row>
-    <row r="335" spans="8:8" s="47" customFormat="1">
-      <c r="H335" s="45"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -3427,298 +3407,172 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="17" collapsed="1"/>
-    <col min="2" max="2" width="10.7109375" style="17" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.28515625" style="17" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.7109375" style="17" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="10" style="17" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21" style="17" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.5703125" style="17" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="24.85546875" style="17" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="9.140625" style="17" collapsed="1"/>
-    <col min="11" max="11" width="14.7109375" style="17" customWidth="1" collapsed="1"/>
-    <col min="12" max="13" width="14" style="17" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="22.42578125" style="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="16384" width="9.140625" style="17" collapsed="1"/>
+    <col min="2" max="2" width="11" style="17" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.5703125" style="17" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="10" style="17" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="21" style="17" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="24.85546875" style="17" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.28515625" style="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.7109375" style="17" customWidth="1" collapsed="1"/>
+    <col min="10" max="11" width="14" style="17" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="22.42578125" style="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="15" width="9.140625" style="17"/>
+    <col min="16" max="16384" width="9.140625" style="17" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="3" customFormat="1" ht="21.75" customHeight="1">
+    <row r="1" spans="1:12" s="3" customFormat="1" ht="21.75" customHeight="1">
       <c r="A1" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>0</v>
+        <v>144</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>151</v>
+        <v>14</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>28</v>
+        <v>257</v>
       </c>
       <c r="I1" s="19" t="s">
-        <v>14</v>
+        <v>133</v>
       </c>
       <c r="J1" s="19" t="s">
-        <v>81</v>
+        <v>145</v>
       </c>
       <c r="K1" s="19" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="L1" s="19" t="s">
-        <v>155</v>
-      </c>
-      <c r="M1" s="19" t="s">
-        <v>159</v>
-      </c>
-      <c r="N1" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" s="16" customFormat="1" ht="21.75" customHeight="1">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="16" customFormat="1" ht="21.75" customHeight="1">
       <c r="A2" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="34" t="s">
-        <v>148</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="34" t="s">
+        <v>260</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="D2" t="s">
+        <v>254</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="F2" s="34" t="s">
+        <v>256</v>
+      </c>
+      <c r="G2" t="s">
         <v>142</v>
       </c>
-      <c r="F2" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="G2" t="s">
-        <v>149</v>
-      </c>
-      <c r="H2" t="s">
-        <v>150</v>
-      </c>
-      <c r="I2" t="s">
-        <v>149</v>
+      <c r="H2" s="14" t="s">
+        <v>258</v>
+      </c>
+      <c r="I2" s="14">
+        <v>90001</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>84</v>
+        <v>146</v>
       </c>
       <c r="K2" s="14">
-        <v>90001</v>
+        <v>64</v>
       </c>
       <c r="L2" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="M2" s="14">
-        <v>64</v>
-      </c>
-      <c r="N2" s="14" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="21.75" customHeight="1">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="21.75" customHeight="1">
       <c r="A3" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>148</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="G3" t="s">
-        <v>149</v>
-      </c>
-      <c r="H3" t="s">
-        <v>150</v>
-      </c>
-      <c r="I3" t="s">
-        <v>149</v>
-      </c>
-      <c r="J3" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="K3" s="14">
-        <v>201301</v>
-      </c>
-      <c r="L3" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="M3" s="14">
-        <v>54</v>
-      </c>
-      <c r="N3" s="14" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="21.75" customHeight="1">
+        <v>7</v>
+      </c>
+      <c r="B3"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="15"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+    </row>
+    <row r="4" spans="1:12" ht="21.75" customHeight="1">
       <c r="A4" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>148</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="G4" t="s">
-        <v>149</v>
-      </c>
-      <c r="H4" t="s">
-        <v>150</v>
-      </c>
-      <c r="I4" t="s">
-        <v>149</v>
-      </c>
-      <c r="J4" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="K4" s="14">
-        <v>90001</v>
-      </c>
-      <c r="L4" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="M4" s="14">
-        <v>69</v>
-      </c>
-      <c r="N4" s="14" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" s="16" customFormat="1" ht="21.75" customHeight="1">
+        <v>12</v>
+      </c>
+      <c r="B4"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="15"/>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+    </row>
+    <row r="5" spans="1:12" s="16" customFormat="1" ht="21.75" customHeight="1">
       <c r="A5" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>148</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="G5" t="s">
-        <v>149</v>
-      </c>
-      <c r="H5" t="s">
-        <v>150</v>
-      </c>
-      <c r="I5" t="s">
-        <v>149</v>
-      </c>
-      <c r="J5" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="K5" s="14">
-        <v>10012</v>
-      </c>
-      <c r="L5" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="M5" s="14">
-        <v>70</v>
-      </c>
-      <c r="N5" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="21.75" customHeight="1">
+        <v>16</v>
+      </c>
+      <c r="B5"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="15"/>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+    </row>
+    <row r="6" spans="1:12" ht="21.75" customHeight="1">
       <c r="A6" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>148</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="G6" t="s">
-        <v>149</v>
-      </c>
-      <c r="H6" t="s">
-        <v>150</v>
-      </c>
-      <c r="I6" t="s">
-        <v>149</v>
-      </c>
-      <c r="J6" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="K6" s="14">
-        <v>10012</v>
-      </c>
-      <c r="L6" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="M6" s="14">
-        <v>72</v>
-      </c>
-      <c r="N6" s="14" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="15" customHeight="1">
-      <c r="A7" s="14"/>
+        <v>88</v>
+      </c>
+      <c r="B6"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="15"/>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+    </row>
+    <row r="7" spans="1:12" ht="15" customHeight="1">
+      <c r="A7" s="14" t="s">
+        <v>243</v>
+      </c>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -3729,16 +3583,60 @@
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
       <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="14" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="14" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="14" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="14" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="14" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="14" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="14" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="14" t="s">
+        <v>252</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
@@ -3770,22 +3668,22 @@
         <v>6</v>
       </c>
       <c r="B1" s="43" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C1" s="43" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D1" s="43" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E1" s="43" t="s">
         <v>18</v>
       </c>
       <c r="F1" s="40" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="G1" s="40" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="H1" s="43" t="s">
         <v>19</v>
@@ -3799,13 +3697,13 @@
     </row>
     <row r="2" spans="1:10" s="36" customFormat="1">
       <c r="A2" s="36" t="s">
+        <v>154</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="36" t="s">
         <v>166</v>
-      </c>
-      <c r="C2" s="36" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="36" t="s">
-        <v>178</v>
       </c>
       <c r="F2" s="41" t="s">
         <v>13</v>
@@ -3816,13 +3714,13 @@
     </row>
     <row r="3" spans="1:10" s="38" customFormat="1">
       <c r="A3" s="38" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E3" s="38" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="F3" s="42" t="s">
         <v>13</v>
@@ -3833,13 +3731,13 @@
     </row>
     <row r="4" spans="1:10" s="36" customFormat="1">
       <c r="A4" s="36" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E4" s="36" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="F4" s="41" t="s">
         <v>8</v>
@@ -3850,13 +3748,13 @@
     </row>
     <row r="5" spans="1:10" s="38" customFormat="1">
       <c r="A5" s="38" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E5" s="38" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="F5" s="42" t="s">
         <v>8</v>
@@ -3867,13 +3765,13 @@
     </row>
     <row r="6" spans="1:10" s="36" customFormat="1">
       <c r="A6" s="36" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E6" s="36" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="F6" s="41" t="s">
         <v>13</v>
@@ -3884,13 +3782,13 @@
     </row>
     <row r="7" spans="1:10" s="38" customFormat="1">
       <c r="A7" s="38" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E7" s="38" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="F7" s="42" t="s">
         <v>8</v>
@@ -3901,13 +3799,13 @@
     </row>
     <row r="8" spans="1:10" s="36" customFormat="1">
       <c r="A8" s="36" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E8" s="36" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="F8" s="41" t="s">
         <v>13</v>
@@ -3918,13 +3816,13 @@
     </row>
     <row r="9" spans="1:10" s="38" customFormat="1">
       <c r="A9" s="38" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E9" s="38" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="F9" s="42" t="s">
         <v>13</v>
@@ -3935,13 +3833,13 @@
     </row>
     <row r="10" spans="1:10" s="36" customFormat="1">
       <c r="A10" s="36" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E10" s="36" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="F10" s="41" t="s">
         <v>13</v>
@@ -3952,13 +3850,13 @@
     </row>
     <row r="11" spans="1:10" s="38" customFormat="1">
       <c r="A11" s="38" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="C11" s="36" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E11" s="38" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="F11" s="42" t="s">
         <v>13</v>
@@ -3969,13 +3867,13 @@
     </row>
     <row r="12" spans="1:10" s="36" customFormat="1">
       <c r="A12" s="36" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="C12" s="36" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E12" s="36" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="F12" s="41" t="s">
         <v>8</v>
@@ -3986,13 +3884,13 @@
     </row>
     <row r="13" spans="1:10" s="38" customFormat="1">
       <c r="A13" s="38" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="C13" s="36" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E13" s="38" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="F13" s="42" t="s">
         <v>13</v>
@@ -4003,13 +3901,13 @@
     </row>
     <row r="14" spans="1:10" s="36" customFormat="1">
       <c r="A14" s="36" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="C14" s="36" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E14" s="36" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="F14" s="41" t="s">
         <v>8</v>
@@ -4020,13 +3918,13 @@
     </row>
     <row r="15" spans="1:10" s="38" customFormat="1">
       <c r="A15" s="38" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="C15" s="36" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E15" s="38" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="F15" s="41" t="s">
         <v>8</v>
@@ -4037,13 +3935,13 @@
     </row>
     <row r="16" spans="1:10" s="36" customFormat="1">
       <c r="A16" s="36" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="C16" s="36" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E16" s="36" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="F16" s="41" t="s">
         <v>8</v>
@@ -4054,13 +3952,13 @@
     </row>
     <row r="17" spans="1:7" s="38" customFormat="1">
       <c r="A17" s="38" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="C17" s="36" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E17" s="38" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="F17" s="42" t="s">
         <v>13</v>
@@ -4071,13 +3969,13 @@
     </row>
     <row r="18" spans="1:7" s="36" customFormat="1">
       <c r="A18" s="36" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="C18" s="36" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E18" s="36" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="F18" s="41" t="s">
         <v>13</v>
@@ -4088,13 +3986,13 @@
     </row>
     <row r="19" spans="1:7" s="38" customFormat="1">
       <c r="A19" s="38" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="C19" s="36" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E19" s="38" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="F19" s="42" t="s">
         <v>13</v>
@@ -4105,13 +4003,13 @@
     </row>
     <row r="20" spans="1:7" s="36" customFormat="1">
       <c r="A20" s="36" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="C20" s="36" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E20" s="36" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="F20" s="41" t="s">
         <v>13</v>
@@ -4122,13 +4020,13 @@
     </row>
     <row r="21" spans="1:7" s="38" customFormat="1">
       <c r="A21" s="38" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="C21" s="36" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E21" s="38" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="F21" s="42" t="s">
         <v>8</v>
@@ -4139,13 +4037,13 @@
     </row>
     <row r="22" spans="1:7" s="36" customFormat="1">
       <c r="A22" s="36" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="C22" s="36" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E22" s="36" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="F22" s="41" t="s">
         <v>8</v>
@@ -4156,13 +4054,13 @@
     </row>
     <row r="23" spans="1:7" s="38" customFormat="1">
       <c r="A23" s="38" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="C23" s="36" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E23" s="38" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="F23" s="42" t="s">
         <v>8</v>
@@ -4173,13 +4071,13 @@
     </row>
     <row r="24" spans="1:7" s="36" customFormat="1">
       <c r="A24" s="36" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C24" s="36" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E24" s="36" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="F24" s="41" t="s">
         <v>13</v>
@@ -4190,13 +4088,13 @@
     </row>
     <row r="25" spans="1:7" s="38" customFormat="1">
       <c r="A25" s="38" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="C25" s="36" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E25" s="38" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="F25" s="42" t="s">
         <v>8</v>
@@ -4207,13 +4105,13 @@
     </row>
     <row r="26" spans="1:7" s="36" customFormat="1">
       <c r="A26" s="36" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="C26" s="36" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E26" s="36" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="F26" s="41" t="s">
         <v>8</v>
@@ -4224,47 +4122,47 @@
     </row>
     <row r="27" spans="1:7" s="38" customFormat="1">
       <c r="A27" s="38" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="C27" s="36" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E27" s="38" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="F27" s="42" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G27" s="42" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:7" s="36" customFormat="1">
       <c r="A28" s="36" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="C28" s="36" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E28" s="36" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="F28" s="41" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G28" s="41" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:7" s="38" customFormat="1">
       <c r="A29" s="38" t="s">
+        <v>229</v>
+      </c>
+      <c r="C29" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29" s="38" t="s">
         <v>241</v>
-      </c>
-      <c r="C29" s="36" t="s">
-        <v>37</v>
-      </c>
-      <c r="E29" s="38" t="s">
-        <v>253</v>
       </c>
       <c r="F29" s="42" t="s">
         <v>13</v>
@@ -4445,19 +4343,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="12.75" customHeight="1">
       <c r="A1" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="B1" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="C1" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="D1" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="E1" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -4482,249 +4380,249 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E1" s="14" t="s">
         <v>5</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="G1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="G2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B3" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="G3" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B4" s="19" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="G4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B5" s="19" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="G5" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="21" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="G6" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="21" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="G7" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B8" s="19" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="21" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="G8" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E9" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="G9" t="s">
         <v>84</v>
-      </c>
-      <c r="F9" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="G9" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E10" s="14">
         <v>90001</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="G10" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B11" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="19" t="s">
-        <v>88</v>
-      </c>
       <c r="D11" s="19" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="G11" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -4749,108 +4647,108 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75">
       <c r="A1" s="22" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C1" s="22" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F1" s="23" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G1" s="23" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="H1" s="33" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18">
       <c r="A2" s="24" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="F2" s="25"/>
       <c r="G2" s="25"/>
     </row>
     <row r="3" spans="1:8" ht="18">
       <c r="A3" s="24" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B3" s="24" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E3" s="25" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="G3" s="25"/>
     </row>
     <row r="4" spans="1:8" ht="18">
       <c r="A4" s="24" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E4" s="25" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="F4" s="25"/>
       <c r="G4" s="25"/>
     </row>
     <row r="5" spans="1:8" ht="18">
       <c r="A5" s="24" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="F5" s="25"/>
       <c r="G5" s="25" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="18">
@@ -4858,13 +4756,13 @@
         <v>0</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E6" s="25" t="s">
         <v>0</v>
@@ -4879,13 +4777,13 @@
         <v>0</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E7" s="25"/>
       <c r="F7" s="25"/>
@@ -4893,58 +4791,58 @@
     </row>
     <row r="8" spans="1:8" ht="18">
       <c r="A8" s="24" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F8" s="25"/>
       <c r="G8" s="25" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="18">
       <c r="A9" s="24" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="F9" s="25"/>
       <c r="G9" s="25" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="18">
       <c r="A10" s="27" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E10" s="28"/>
       <c r="F10" s="28"/>
@@ -4952,16 +4850,16 @@
     </row>
     <row r="11" spans="1:8" ht="18">
       <c r="A11" s="27" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E11" s="28"/>
       <c r="F11" s="28"/>
@@ -4969,16 +4867,16 @@
     </row>
     <row r="12" spans="1:8" ht="18">
       <c r="A12" s="27" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E12" s="28"/>
       <c r="F12" s="28"/>
@@ -4989,13 +4887,13 @@
         <v>0</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E13" s="28"/>
       <c r="F13" s="28"/>
@@ -5003,12 +4901,12 @@
     </row>
     <row r="14" spans="1:8" ht="18">
       <c r="A14" s="27" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B14" s="27"/>
       <c r="C14" s="28"/>
       <c r="D14" s="29" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E14" s="28"/>
       <c r="F14" s="28"/>
@@ -5016,12 +4914,12 @@
     </row>
     <row r="15" spans="1:8" ht="18">
       <c r="A15" s="27" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B15" s="27"/>
       <c r="C15" s="28"/>
       <c r="D15" s="29" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E15" s="28"/>
       <c r="F15" s="28"/>
@@ -5029,12 +4927,12 @@
     </row>
     <row r="16" spans="1:8" ht="18">
       <c r="A16" s="27" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B16" s="27"/>
       <c r="C16" s="28"/>
       <c r="D16" s="29" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
@@ -5042,12 +4940,12 @@
     </row>
     <row r="17" spans="1:7" ht="18">
       <c r="A17" s="27" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B17" s="27"/>
       <c r="C17" s="28"/>
       <c r="D17" s="29" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E17" s="28"/>
       <c r="F17" s="28"/>

</xml_diff>